<commit_message>
ID for cards starts with 0
</commit_message>
<xml_diff>
--- a/card_info.xlsx
+++ b/card_info.xlsx
@@ -3208,8 +3208,8 @@
   <dimension ref="A1:J482"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A459" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B482" sqref="B482"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3260,7 +3260,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>139</v>
@@ -3288,7 +3288,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>106</v>
@@ -3320,7 +3320,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>84</v>
@@ -3350,7 +3350,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>34</v>
@@ -3380,7 +3380,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>56</v>
@@ -3410,7 +3410,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>108</v>
@@ -3442,7 +3442,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>141</v>
@@ -3472,7 +3472,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>158</v>
@@ -3502,7 +3502,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>162</v>
@@ -3532,7 +3532,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>168</v>
@@ -3564,7 +3564,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>171</v>
@@ -3594,7 +3594,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>173</v>
@@ -3624,7 +3624,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>177</v>
@@ -3654,7 +3654,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>147</v>
@@ -3686,7 +3686,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>152</v>
@@ -3716,7 +3716,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>156</v>
@@ -3748,7 +3748,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>160</v>
@@ -3778,7 +3778,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>163</v>
@@ -3810,7 +3810,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>165</v>
@@ -3840,7 +3840,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>143</v>
@@ -3872,7 +3872,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>145</v>
@@ -3902,7 +3902,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>150</v>
@@ -3932,7 +3932,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>153</v>
@@ -3964,7 +3964,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>170</v>
@@ -3996,7 +3996,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>18</v>
@@ -4028,7 +4028,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>175</v>
@@ -4060,7 +4060,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>102</v>
@@ -4092,7 +4092,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>167</v>
@@ -4122,7 +4122,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>183</v>
@@ -4152,7 +4152,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>221</v>
@@ -4182,7 +4182,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>109</v>
@@ -4214,7 +4214,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>179</v>
@@ -4244,7 +4244,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>185</v>
@@ -4274,7 +4274,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>199</v>
@@ -4306,7 +4306,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>205</v>
@@ -4336,7 +4336,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>213</v>
@@ -4366,7 +4366,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>37</v>
@@ -4396,7 +4396,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>234</v>
@@ -4426,7 +4426,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>236</v>
@@ -4456,7 +4456,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>181</v>
@@ -4486,7 +4486,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>188</v>
@@ -4518,7 +4518,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>231</v>
@@ -4548,7 +4548,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>232</v>
@@ -4578,7 +4578,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>47</v>
@@ -4608,7 +4608,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>193</v>
@@ -4638,7 +4638,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>128</v>
@@ -4668,7 +4668,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>71</v>
@@ -4698,7 +4698,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>195</v>
@@ -4730,7 +4730,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>202</v>
@@ -4760,7 +4760,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>207</v>
@@ -4790,7 +4790,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>217</v>
@@ -4820,7 +4820,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>229</v>
@@ -4850,7 +4850,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>22</v>
@@ -4882,7 +4882,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>125</v>
@@ -4912,7 +4912,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>215</v>
@@ -4942,7 +4942,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>219</v>
@@ -4972,7 +4972,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>190</v>
@@ -5004,7 +5004,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>203</v>
@@ -5036,7 +5036,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>209</v>
@@ -5066,7 +5066,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>223</v>
@@ -5098,7 +5098,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>24</v>
@@ -5130,7 +5130,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>186</v>
@@ -5160,7 +5160,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>191</v>
@@ -5192,7 +5192,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>227</v>
@@ -5222,7 +5222,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>74</v>
@@ -5252,7 +5252,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>197</v>
@@ -5282,7 +5282,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>87</v>
@@ -5314,7 +5314,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>59</v>
@@ -5344,7 +5344,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>211</v>
@@ -5374,7 +5374,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>225</v>
@@ -5404,7 +5404,7 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>265</v>
@@ -5434,7 +5434,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>270</v>
@@ -5466,7 +5466,7 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>111</v>
@@ -5498,7 +5498,7 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>39</v>
@@ -5528,7 +5528,7 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>50</v>
@@ -5558,7 +5558,7 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>246</v>
@@ -5588,7 +5588,7 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>255</v>
@@ -5618,7 +5618,7 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>268</v>
@@ -5650,7 +5650,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>273</v>
@@ -5680,7 +5680,7 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>275</v>
@@ -5712,7 +5712,7 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>279</v>
@@ -5742,7 +5742,7 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>78</v>
@@ -5772,7 +5772,7 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>289</v>
@@ -5804,7 +5804,7 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>294</v>
@@ -5834,7 +5834,7 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>113</v>
@@ -5866,7 +5866,7 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>242</v>
@@ -5896,7 +5896,7 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>244</v>
@@ -5926,7 +5926,7 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>269</v>
@@ -5958,7 +5958,7 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>130</v>
@@ -5988,7 +5988,7 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>92</v>
@@ -6018,7 +6018,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>286</v>
@@ -6048,7 +6048,7 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>250</v>
@@ -6080,7 +6080,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>257</v>
@@ -6112,7 +6112,7 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>259</v>
@@ -6142,7 +6142,7 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>261</v>
@@ -6172,7 +6172,7 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>283</v>
@@ -6202,7 +6202,7 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>291</v>
@@ -6232,7 +6232,7 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>293</v>
@@ -6262,7 +6262,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>132</v>
@@ -6292,7 +6292,7 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>272</v>
@@ -6320,7 +6320,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>263</v>
@@ -6350,7 +6350,7 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>248</v>
@@ -6382,7 +6382,7 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>76</v>
@@ -6412,7 +6412,7 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>267</v>
@@ -6442,7 +6442,7 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>277</v>
@@ -6472,7 +6472,7 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>281</v>
@@ -6502,7 +6502,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>252</v>
@@ -6532,7 +6532,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>253</v>
@@ -6562,7 +6562,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>288</v>
@@ -6594,7 +6594,7 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>285</v>
@@ -6624,7 +6624,7 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>296</v>
@@ -6654,7 +6654,7 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>238</v>
@@ -6684,7 +6684,7 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>240</v>
@@ -6714,7 +6714,7 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>90</v>
@@ -6746,7 +6746,7 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>115</v>
@@ -6778,7 +6778,7 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>297</v>
@@ -6808,7 +6808,7 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>300</v>
@@ -6836,7 +6836,7 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>43</v>
@@ -6866,7 +6866,7 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>303</v>
@@ -6896,7 +6896,7 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>80</v>
@@ -6926,7 +6926,7 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>315</v>
@@ -6956,7 +6956,7 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>61</v>
@@ -6986,7 +6986,7 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>318</v>
@@ -7016,7 +7016,7 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>324</v>
@@ -7046,7 +7046,7 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>314</v>
@@ -7076,7 +7076,7 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>311</v>
@@ -7106,7 +7106,7 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>26</v>
@@ -7136,7 +7136,7 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>136</v>
@@ -7166,7 +7166,7 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>320</v>
@@ -7196,7 +7196,7 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>298</v>
@@ -7226,7 +7226,7 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>321</v>
@@ -7256,7 +7256,7 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>134</v>
@@ -7286,7 +7286,7 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>308</v>
@@ -7318,7 +7318,7 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>41</v>
@@ -7348,7 +7348,7 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>319</v>
@@ -7378,7 +7378,7 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>94</v>
@@ -7408,7 +7408,7 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>301</v>
@@ -7438,7 +7438,7 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>306</v>
@@ -7468,7 +7468,7 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>310</v>
@@ -7498,7 +7498,7 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>0</v>
@@ -7528,7 +7528,7 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>316</v>
@@ -7560,7 +7560,7 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>313</v>
@@ -7590,7 +7590,7 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>304</v>
@@ -7620,7 +7620,7 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>322</v>
@@ -7652,7 +7652,7 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>63</v>
@@ -7682,7 +7682,7 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>117</v>
@@ -7712,7 +7712,7 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>96</v>
@@ -7742,7 +7742,7 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>359</v>
@@ -7772,7 +7772,7 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>119</v>
@@ -7804,7 +7804,7 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>335</v>
@@ -7834,7 +7834,7 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>358</v>
@@ -7866,7 +7866,7 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>352</v>
@@ -7896,7 +7896,7 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>330</v>
@@ -7926,7 +7926,7 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>331</v>
@@ -7958,7 +7958,7 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>346</v>
@@ -7988,7 +7988,7 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B157" s="2" t="s">
         <v>333</v>
@@ -8018,7 +8018,7 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B158" s="2" t="s">
         <v>339</v>
@@ -8048,7 +8048,7 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B159" s="2" t="s">
         <v>326</v>
@@ -8078,7 +8078,7 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>328</v>
@@ -8110,7 +8110,7 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>4</v>
@@ -8140,7 +8140,7 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B162" s="2" t="s">
         <v>340</v>
@@ -8170,7 +8170,7 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B163" s="2" t="s">
         <v>342</v>
@@ -8200,7 +8200,7 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B164" s="2" t="s">
         <v>348</v>
@@ -8230,7 +8230,7 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>350</v>
@@ -8260,7 +8260,7 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>354</v>
@@ -8292,7 +8292,7 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>344</v>
@@ -8322,7 +8322,7 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B168" s="2" t="s">
         <v>28</v>
@@ -8354,7 +8354,7 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>337</v>
@@ -8384,7 +8384,7 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>356</v>
@@ -8414,7 +8414,7 @@
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>383</v>
@@ -8446,7 +8446,7 @@
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>364</v>
@@ -8474,7 +8474,7 @@
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>121</v>
@@ -8506,7 +8506,7 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B174" s="2" t="s">
         <v>369</v>
@@ -8536,7 +8536,7 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>67</v>
@@ -8566,7 +8566,7 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B176" s="2" t="s">
         <v>373</v>
@@ -8598,7 +8598,7 @@
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B177" s="2" t="s">
         <v>98</v>
@@ -8628,7 +8628,7 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>375</v>
@@ -8658,7 +8658,7 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B179" s="2" t="s">
         <v>30</v>
@@ -8690,7 +8690,7 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>361</v>
@@ -8720,7 +8720,7 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B181" s="2" t="s">
         <v>367</v>
@@ -8750,7 +8750,7 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B182" s="2" t="s">
         <v>381</v>
@@ -8780,7 +8780,7 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B183" s="2" t="s">
         <v>376</v>
@@ -8810,7 +8810,7 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B184" s="2" t="s">
         <v>65</v>
@@ -8840,7 +8840,7 @@
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B185" s="2" t="s">
         <v>365</v>
@@ -8870,7 +8870,7 @@
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B186" s="2" t="s">
         <v>379</v>
@@ -8900,7 +8900,7 @@
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B187" s="2" t="s">
         <v>385</v>
@@ -8930,7 +8930,7 @@
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B188" s="2" t="s">
         <v>387</v>
@@ -8960,7 +8960,7 @@
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B189" s="2" t="s">
         <v>371</v>
@@ -8990,7 +8990,7 @@
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>82</v>
@@ -9020,7 +9020,7 @@
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>378</v>
@@ -9050,7 +9050,7 @@
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B192" s="2" t="s">
         <v>362</v>
@@ -9080,7 +9080,7 @@
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B193" s="2" t="s">
         <v>69</v>
@@ -9110,7 +9110,7 @@
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B194" s="2" t="s">
         <v>394</v>
@@ -9138,7 +9138,7 @@
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B195" s="2" t="s">
         <v>390</v>
@@ -9168,7 +9168,7 @@
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B196" s="2" t="s">
         <v>392</v>
@@ -9198,7 +9198,7 @@
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B197" s="2" t="s">
         <v>388</v>
@@ -9228,7 +9228,7 @@
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B198" s="2" t="s">
         <v>391</v>
@@ -9258,7 +9258,7 @@
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>45</v>
@@ -9288,7 +9288,7 @@
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>52</v>
@@ -9318,7 +9318,7 @@
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B201" s="2" t="s">
         <v>7</v>
@@ -9348,7 +9348,7 @@
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B202" s="2" t="s">
         <v>10</v>
@@ -9378,7 +9378,7 @@
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>12</v>
@@ -9408,7 +9408,7 @@
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>397</v>
@@ -9438,7 +9438,7 @@
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>395</v>
@@ -9468,7 +9468,7 @@
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>54</v>
@@ -9498,7 +9498,7 @@
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>137</v>
@@ -9528,7 +9528,7 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B208" s="2" t="s">
         <v>100</v>
@@ -9558,7 +9558,7 @@
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B209" s="2" t="s">
         <v>399</v>
@@ -9590,7 +9590,7 @@
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B210" s="2" t="s">
         <v>32</v>
@@ -9622,7 +9622,7 @@
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B211" s="2" t="s">
         <v>403</v>
@@ -9654,7 +9654,7 @@
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B212" s="2" t="s">
         <v>405</v>
@@ -9686,7 +9686,7 @@
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B213" s="2" t="s">
         <v>401</v>
@@ -9718,7 +9718,7 @@
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B214" s="2" t="s">
         <v>407</v>
@@ -9750,7 +9750,7 @@
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>123</v>
@@ -9782,7 +9782,7 @@
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B216" s="2" t="s">
         <v>15</v>
@@ -9812,7 +9812,7 @@
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B217" s="2" t="s">
         <v>409</v>
@@ -9844,7 +9844,7 @@
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B218" s="2" t="s">
         <v>411</v>
@@ -9874,7 +9874,7 @@
     </row>
     <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B219" s="2" t="s">
         <v>413</v>
@@ -9904,7 +9904,7 @@
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B220" s="2" t="s">
         <v>415</v>
@@ -9934,7 +9934,7 @@
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B221" s="2" t="s">
         <v>536</v>
@@ -9957,7 +9957,7 @@
     </row>
     <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B222" s="2" t="s">
         <v>538</v>
@@ -9980,7 +9980,7 @@
     </row>
     <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>540</v>
@@ -10003,7 +10003,7 @@
     </row>
     <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>542</v>
@@ -10026,7 +10026,7 @@
     </row>
     <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B225" s="2" t="s">
         <v>544</v>
@@ -10049,7 +10049,7 @@
     </row>
     <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B226" s="2" t="s">
         <v>546</v>
@@ -10072,7 +10072,7 @@
     </row>
     <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B227" s="2" t="s">
         <v>548</v>
@@ -10095,7 +10095,7 @@
     </row>
     <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B228" s="2" t="s">
         <v>550</v>
@@ -10118,7 +10118,7 @@
     </row>
     <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B229" s="2" t="s">
         <v>552</v>
@@ -10141,7 +10141,7 @@
     </row>
     <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B230" s="2" t="s">
         <v>554</v>
@@ -10164,7 +10164,7 @@
     </row>
     <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B231" s="2" t="s">
         <v>556</v>
@@ -10187,7 +10187,7 @@
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B232" s="2" t="s">
         <v>558</v>
@@ -10210,7 +10210,7 @@
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B233" s="2" t="s">
         <v>560</v>
@@ -10233,7 +10233,7 @@
     </row>
     <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B234" s="2" t="s">
         <v>562</v>
@@ -10256,7 +10256,7 @@
     </row>
     <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B235" s="2" t="s">
         <v>564</v>
@@ -10279,7 +10279,7 @@
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B236" s="2" t="s">
         <v>566</v>
@@ -10302,7 +10302,7 @@
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B237" s="2" t="s">
         <v>568</v>
@@ -10325,7 +10325,7 @@
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B238" s="2" t="s">
         <v>570</v>
@@ -10348,7 +10348,7 @@
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B239" s="2" t="s">
         <v>572</v>
@@ -10371,7 +10371,7 @@
     </row>
     <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B240" s="2" t="s">
         <v>574</v>
@@ -10394,7 +10394,7 @@
     </row>
     <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B241" s="2" t="s">
         <v>576</v>
@@ -10417,7 +10417,7 @@
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B242" s="2" t="s">
         <v>578</v>
@@ -10440,7 +10440,7 @@
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B243" s="2" t="s">
         <v>580</v>
@@ -10463,7 +10463,7 @@
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B244" s="2" t="s">
         <v>582</v>
@@ -10486,7 +10486,7 @@
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B245" s="4" t="s">
         <v>584</v>
@@ -10509,7 +10509,7 @@
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B246" s="4" t="s">
         <v>586</v>
@@ -10532,7 +10532,7 @@
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B247" s="4" t="s">
         <v>588</v>
@@ -10555,7 +10555,7 @@
     </row>
     <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B248" s="4" t="s">
         <v>590</v>
@@ -10578,7 +10578,7 @@
     </row>
     <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B249" s="4" t="s">
         <v>592</v>
@@ -10601,7 +10601,7 @@
     </row>
     <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B250" s="2" t="s">
         <v>594</v>
@@ -10624,7 +10624,7 @@
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B251" s="2" t="s">
         <v>596</v>
@@ -10647,7 +10647,7 @@
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B252" s="2" t="s">
         <v>598</v>
@@ -10670,7 +10670,7 @@
     </row>
     <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B253" s="2" t="s">
         <v>600</v>
@@ -10693,7 +10693,7 @@
     </row>
     <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B254" s="2" t="s">
         <v>602</v>
@@ -10716,7 +10716,7 @@
     </row>
     <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B255" s="2" t="s">
         <v>604</v>
@@ -10739,7 +10739,7 @@
     </row>
     <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B256" s="2" t="s">
         <v>606</v>
@@ -10762,7 +10762,7 @@
     </row>
     <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B257" s="2" t="s">
         <v>608</v>
@@ -10785,7 +10785,7 @@
     </row>
     <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B258" s="2" t="s">
         <v>422</v>
@@ -10808,7 +10808,7 @@
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B259" s="2" t="s">
         <v>611</v>
@@ -10831,7 +10831,7 @@
     </row>
     <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B260" s="2" t="s">
         <v>613</v>
@@ -10854,7 +10854,7 @@
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B261" s="2" t="s">
         <v>615</v>
@@ -10877,7 +10877,7 @@
     </row>
     <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B262" s="2" t="s">
         <v>617</v>
@@ -10900,7 +10900,7 @@
     </row>
     <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B263" s="2" t="s">
         <v>619</v>
@@ -10923,7 +10923,7 @@
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>621</v>
@@ -10946,7 +10946,7 @@
     </row>
     <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B265" s="2" t="s">
         <v>623</v>
@@ -10969,7 +10969,7 @@
     </row>
     <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B266" s="2" t="s">
         <v>625</v>
@@ -10992,7 +10992,7 @@
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B267" s="2" t="s">
         <v>432</v>
@@ -11015,7 +11015,7 @@
     </row>
     <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B268" s="2" t="s">
         <v>628</v>
@@ -11038,7 +11038,7 @@
     </row>
     <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B269" s="2" t="s">
         <v>630</v>
@@ -11061,7 +11061,7 @@
     </row>
     <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B270" s="2" t="s">
         <v>632</v>
@@ -11084,7 +11084,7 @@
     </row>
     <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B271" s="2" t="s">
         <v>634</v>
@@ -11107,7 +11107,7 @@
     </row>
     <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B272" s="2" t="s">
         <v>636</v>
@@ -11130,7 +11130,7 @@
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B273" s="2" t="s">
         <v>638</v>
@@ -11153,7 +11153,7 @@
     </row>
     <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B274" s="2" t="s">
         <v>640</v>
@@ -11176,7 +11176,7 @@
     </row>
     <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B275" s="2" t="s">
         <v>642</v>
@@ -11199,7 +11199,7 @@
     </row>
     <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B276" s="2" t="s">
         <v>644</v>
@@ -11222,7 +11222,7 @@
     </row>
     <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B277" s="2" t="s">
         <v>646</v>
@@ -11245,7 +11245,7 @@
     </row>
     <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B278" s="2" t="s">
         <v>648</v>
@@ -11268,7 +11268,7 @@
     </row>
     <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B279" s="2" t="s">
         <v>650</v>
@@ -11291,7 +11291,7 @@
     </row>
     <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B280" s="2" t="s">
         <v>652</v>
@@ -11314,7 +11314,7 @@
     </row>
     <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B281" s="2" t="s">
         <v>654</v>
@@ -11337,7 +11337,7 @@
     </row>
     <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B282" s="2" t="s">
         <v>656</v>
@@ -11360,7 +11360,7 @@
     </row>
     <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B283" s="2" t="s">
         <v>658</v>
@@ -11383,7 +11383,7 @@
     </row>
     <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B284" s="2" t="s">
         <v>660</v>
@@ -11406,7 +11406,7 @@
     </row>
     <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B285" s="2" t="s">
         <v>662</v>
@@ -11429,7 +11429,7 @@
     </row>
     <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B286" s="2" t="s">
         <v>664</v>
@@ -11452,7 +11452,7 @@
     </row>
     <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B287" s="2" t="s">
         <v>666</v>
@@ -11475,7 +11475,7 @@
     </row>
     <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B288" s="2" t="s">
         <v>668</v>
@@ -11498,7 +11498,7 @@
     </row>
     <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B289" s="2" t="s">
         <v>670</v>
@@ -11521,7 +11521,7 @@
     </row>
     <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B290" s="2" t="s">
         <v>672</v>
@@ -11544,7 +11544,7 @@
     </row>
     <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B291" s="2" t="s">
         <v>674</v>
@@ -11567,7 +11567,7 @@
     </row>
     <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B292" s="2" t="s">
         <v>676</v>
@@ -11590,7 +11590,7 @@
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B293" s="2" t="s">
         <v>678</v>
@@ -11613,7 +11613,7 @@
     </row>
     <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B294" s="2" t="s">
         <v>680</v>
@@ -11636,7 +11636,7 @@
     </row>
     <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B295" s="2" t="s">
         <v>682</v>
@@ -11659,7 +11659,7 @@
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B296" s="2" t="s">
         <v>683</v>
@@ -11682,7 +11682,7 @@
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B297" s="2" t="s">
         <v>685</v>
@@ -11705,7 +11705,7 @@
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B298" s="2" t="s">
         <v>687</v>
@@ -11728,7 +11728,7 @@
     </row>
     <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B299" s="2" t="s">
         <v>689</v>
@@ -11751,7 +11751,7 @@
     </row>
     <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B300" s="2" t="s">
         <v>691</v>
@@ -11774,7 +11774,7 @@
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B301" s="2" t="s">
         <v>693</v>
@@ -11797,7 +11797,7 @@
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B302" s="2" t="s">
         <v>695</v>
@@ -11820,7 +11820,7 @@
     </row>
     <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B303" s="2" t="s">
         <v>697</v>
@@ -11843,7 +11843,7 @@
     </row>
     <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B304" s="2" t="s">
         <v>699</v>
@@ -11866,7 +11866,7 @@
     </row>
     <row r="305" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B305" s="2" t="s">
         <v>701</v>
@@ -11889,7 +11889,7 @@
     </row>
     <row r="306" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B306" s="2" t="s">
         <v>703</v>
@@ -11912,7 +11912,7 @@
     </row>
     <row r="307" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B307" s="2" t="s">
         <v>705</v>
@@ -11935,7 +11935,7 @@
     </row>
     <row r="308" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B308" s="2" t="s">
         <v>707</v>
@@ -11958,7 +11958,7 @@
     </row>
     <row r="309" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B309" s="5" t="s">
         <v>709</v>
@@ -11981,7 +11981,7 @@
     </row>
     <row r="310" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B310" s="5" t="s">
         <v>711</v>
@@ -12004,7 +12004,7 @@
     </row>
     <row r="311" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B311" s="2" t="s">
         <v>713</v>
@@ -12027,7 +12027,7 @@
     </row>
     <row r="312" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B312" s="2" t="s">
         <v>715</v>
@@ -12050,7 +12050,7 @@
     </row>
     <row r="313" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B313" s="2" t="s">
         <v>717</v>
@@ -12073,7 +12073,7 @@
     </row>
     <row r="314" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B314" s="2" t="s">
         <v>719</v>
@@ -12096,7 +12096,7 @@
     </row>
     <row r="315" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B315" s="2" t="s">
         <v>721</v>
@@ -12119,7 +12119,7 @@
     </row>
     <row r="316" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B316" s="2" t="s">
         <v>723</v>
@@ -12142,7 +12142,7 @@
     </row>
     <row r="317" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B317" s="2" t="s">
         <v>725</v>
@@ -12165,7 +12165,7 @@
     </row>
     <row r="318" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B318" s="2" t="s">
         <v>727</v>
@@ -12188,7 +12188,7 @@
     </row>
     <row r="319" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B319" s="2" t="s">
         <v>729</v>
@@ -12211,7 +12211,7 @@
     </row>
     <row r="320" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B320" s="2" t="s">
         <v>731</v>
@@ -12234,7 +12234,7 @@
     </row>
     <row r="321" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B321" s="2" t="s">
         <v>733</v>
@@ -12257,7 +12257,7 @@
     </row>
     <row r="322" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B322" s="2" t="s">
         <v>735</v>
@@ -12280,7 +12280,7 @@
     </row>
     <row r="323" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B323" s="2" t="s">
         <v>737</v>
@@ -12303,7 +12303,7 @@
     </row>
     <row r="324" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B324" s="2" t="s">
         <v>739</v>
@@ -12326,7 +12326,7 @@
     </row>
     <row r="325" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B325" s="2" t="s">
         <v>741</v>
@@ -12349,7 +12349,7 @@
     </row>
     <row r="326" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B326" s="2" t="s">
         <v>743</v>
@@ -12372,7 +12372,7 @@
     </row>
     <row r="327" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B327" s="2" t="s">
         <v>745</v>
@@ -12395,7 +12395,7 @@
     </row>
     <row r="328" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B328" s="2" t="s">
         <v>747</v>
@@ -12418,7 +12418,7 @@
     </row>
     <row r="329" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B329" s="2" t="s">
         <v>749</v>
@@ -12441,7 +12441,7 @@
     </row>
     <row r="330" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B330" s="2" t="s">
         <v>751</v>
@@ -12464,7 +12464,7 @@
     </row>
     <row r="331" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B331" s="2" t="s">
         <v>753</v>
@@ -12487,7 +12487,7 @@
     </row>
     <row r="332" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B332" s="2" t="s">
         <v>755</v>
@@ -12510,7 +12510,7 @@
     </row>
     <row r="333" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B333" s="2" t="s">
         <v>757</v>
@@ -12533,7 +12533,7 @@
     </row>
     <row r="334" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B334" s="2" t="s">
         <v>759</v>
@@ -12556,7 +12556,7 @@
     </row>
     <row r="335" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B335" s="2" t="s">
         <v>761</v>
@@ -12579,7 +12579,7 @@
     </row>
     <row r="336" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B336" s="2" t="s">
         <v>176</v>
@@ -12602,7 +12602,7 @@
     </row>
     <row r="337" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B337" s="2" t="s">
         <v>764</v>
@@ -12625,7 +12625,7 @@
     </row>
     <row r="338" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B338" s="2" t="s">
         <v>766</v>
@@ -12648,7 +12648,7 @@
     </row>
     <row r="339" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B339" s="2" t="s">
         <v>768</v>
@@ -12671,7 +12671,7 @@
     </row>
     <row r="340" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B340" s="2" t="s">
         <v>770</v>
@@ -12694,7 +12694,7 @@
     </row>
     <row r="341" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B341" s="2" t="s">
         <v>772</v>
@@ -12717,7 +12717,7 @@
     </row>
     <row r="342" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B342" s="2" t="s">
         <v>774</v>
@@ -12740,7 +12740,7 @@
     </row>
     <row r="343" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B343" s="2" t="s">
         <v>776</v>
@@ -12763,7 +12763,7 @@
     </row>
     <row r="344" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B344" s="2" t="s">
         <v>778</v>
@@ -12786,7 +12786,7 @@
     </row>
     <row r="345" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B345" s="2" t="s">
         <v>780</v>
@@ -12809,7 +12809,7 @@
     </row>
     <row r="346" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B346" s="2" t="s">
         <v>782</v>
@@ -12832,7 +12832,7 @@
     </row>
     <row r="347" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B347" s="2" t="s">
         <v>784</v>
@@ -12855,7 +12855,7 @@
     </row>
     <row r="348" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B348" s="2" t="s">
         <v>786</v>
@@ -12878,7 +12878,7 @@
     </row>
     <row r="349" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B349" s="2" t="s">
         <v>788</v>
@@ -12901,7 +12901,7 @@
     </row>
     <row r="350" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B350" s="2" t="s">
         <v>790</v>
@@ -12924,7 +12924,7 @@
     </row>
     <row r="351" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B351" s="2" t="s">
         <v>792</v>
@@ -12947,7 +12947,7 @@
     </row>
     <row r="352" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B352" s="2" t="s">
         <v>794</v>
@@ -12970,7 +12970,7 @@
     </row>
     <row r="353" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B353" s="2" t="s">
         <v>796</v>
@@ -12993,7 +12993,7 @@
     </row>
     <row r="354" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B354" s="2" t="s">
         <v>798</v>
@@ -13016,7 +13016,7 @@
     </row>
     <row r="355" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B355" s="2" t="s">
         <v>800</v>
@@ -13039,7 +13039,7 @@
     </row>
     <row r="356" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A356" s="1">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B356" s="2" t="s">
         <v>802</v>
@@ -13062,7 +13062,7 @@
     </row>
     <row r="357" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A357" s="1">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B357" s="2" t="s">
         <v>804</v>
@@ -13085,7 +13085,7 @@
     </row>
     <row r="358" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A358" s="1">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B358" s="2" t="s">
         <v>806</v>
@@ -13108,7 +13108,7 @@
     </row>
     <row r="359" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A359" s="1">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B359" s="2" t="s">
         <v>808</v>
@@ -13131,7 +13131,7 @@
     </row>
     <row r="360" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B360" s="2" t="s">
         <v>810</v>
@@ -13154,7 +13154,7 @@
     </row>
     <row r="361" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A361" s="1">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B361" s="2" t="s">
         <v>812</v>
@@ -13177,7 +13177,7 @@
     </row>
     <row r="362" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B362" s="2" t="s">
         <v>814</v>
@@ -13200,7 +13200,7 @@
     </row>
     <row r="363" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A363" s="1">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B363" s="2" t="s">
         <v>816</v>
@@ -13223,7 +13223,7 @@
     </row>
     <row r="364" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B364" s="2" t="s">
         <v>818</v>
@@ -13246,7 +13246,7 @@
     </row>
     <row r="365" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A365" s="1">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B365" s="2" t="s">
         <v>820</v>
@@ -13269,7 +13269,7 @@
     </row>
     <row r="366" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B366" s="2" t="s">
         <v>822</v>
@@ -13292,7 +13292,7 @@
     </row>
     <row r="367" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A367" s="1">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B367" s="2" t="s">
         <v>824</v>
@@ -13315,7 +13315,7 @@
     </row>
     <row r="368" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A368" s="1">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B368" s="2" t="s">
         <v>33</v>
@@ -13338,7 +13338,7 @@
     </row>
     <row r="369" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A369" s="1">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B369" s="2" t="s">
         <v>827</v>
@@ -13361,7 +13361,7 @@
     </row>
     <row r="370" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A370" s="1">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B370" s="2" t="s">
         <v>829</v>
@@ -13384,7 +13384,7 @@
     </row>
     <row r="371" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A371" s="1">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B371" s="2" t="s">
         <v>831</v>
@@ -13407,7 +13407,7 @@
     </row>
     <row r="372" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A372" s="1">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B372" s="2" t="s">
         <v>889</v>
@@ -13436,7 +13436,7 @@
     </row>
     <row r="373" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A373" s="1">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B373" s="2" t="s">
         <v>891</v>
@@ -13465,7 +13465,7 @@
     </row>
     <row r="374" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A374" s="1">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B374" s="2" t="s">
         <v>893</v>
@@ -13492,7 +13492,7 @@
     </row>
     <row r="375" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A375" s="1">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B375" s="2" t="s">
         <v>894</v>
@@ -13521,7 +13521,7 @@
     </row>
     <row r="376" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A376" s="1">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B376" s="2" t="s">
         <v>896</v>
@@ -13550,7 +13550,7 @@
     </row>
     <row r="377" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A377" s="1">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B377" s="2" t="s">
         <v>898</v>
@@ -13579,7 +13579,7 @@
     </row>
     <row r="378" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A378" s="1">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B378" s="2" t="s">
         <v>900</v>
@@ -13606,7 +13606,7 @@
     </row>
     <row r="379" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A379" s="1">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B379" s="2" t="s">
         <v>901</v>
@@ -13635,7 +13635,7 @@
     </row>
     <row r="380" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A380" s="1">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B380" s="2" t="s">
         <v>903</v>
@@ -13664,7 +13664,7 @@
     </row>
     <row r="381" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A381" s="1">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B381" s="2" t="s">
         <v>905</v>
@@ -13691,7 +13691,7 @@
     </row>
     <row r="382" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A382" s="1">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B382" s="2" t="s">
         <v>906</v>
@@ -13718,7 +13718,7 @@
     </row>
     <row r="383" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A383" s="1">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B383" s="2" t="s">
         <v>907</v>
@@ -13746,8 +13746,8 @@
       </c>
     </row>
     <row r="384" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A384" s="6">
-        <v>383</v>
+      <c r="A384" s="1">
+        <v>382</v>
       </c>
       <c r="B384" s="7" t="s">
         <v>925</v>
@@ -13770,7 +13770,7 @@
     </row>
     <row r="385" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A385" s="1">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B385" s="7" t="s">
         <v>886</v>
@@ -13793,7 +13793,7 @@
     </row>
     <row r="386" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A386" s="1">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B386" s="7" t="s">
         <v>888</v>
@@ -13816,7 +13816,7 @@
     </row>
     <row r="387" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A387" s="1">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B387" s="7" t="s">
         <v>493</v>
@@ -13848,7 +13848,7 @@
     </row>
     <row r="388" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A388" s="1">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B388" s="7" t="s">
         <v>495</v>
@@ -13880,7 +13880,7 @@
     </row>
     <row r="389" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A389" s="1">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B389" s="7" t="s">
         <v>497</v>
@@ -13912,7 +13912,7 @@
     </row>
     <row r="390" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A390" s="1">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B390" s="7" t="s">
         <v>507</v>
@@ -13944,7 +13944,7 @@
     </row>
     <row r="391" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A391" s="1">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B391" s="7" t="s">
         <v>876</v>
@@ -13967,7 +13967,7 @@
     </row>
     <row r="392" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A392" s="1">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B392" s="7" t="s">
         <v>860</v>
@@ -13990,7 +13990,7 @@
     </row>
     <row r="393" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A393" s="1">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B393" s="7" t="s">
         <v>882</v>
@@ -14013,7 +14013,7 @@
     </row>
     <row r="394" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A394" s="1">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B394" s="7" t="s">
         <v>917</v>
@@ -14042,7 +14042,7 @@
     </row>
     <row r="395" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A395" s="1">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B395" s="7" t="s">
         <v>526</v>
@@ -14071,7 +14071,7 @@
     </row>
     <row r="396" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A396" s="1">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B396" s="7" t="s">
         <v>475</v>
@@ -14103,7 +14103,7 @@
     </row>
     <row r="397" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A397" s="1">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B397" s="7" t="s">
         <v>442</v>
@@ -14132,7 +14132,7 @@
     </row>
     <row r="398" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A398" s="1">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B398" s="7" t="s">
         <v>878</v>
@@ -14155,7 +14155,7 @@
     </row>
     <row r="399" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A399" s="1">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B399" s="7" t="s">
         <v>841</v>
@@ -14178,7 +14178,7 @@
     </row>
     <row r="400" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A400" s="1">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B400" s="7" t="s">
         <v>849</v>
@@ -14201,7 +14201,7 @@
     </row>
     <row r="401" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A401" s="1">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B401" s="7" t="s">
         <v>856</v>
@@ -14224,7 +14224,7 @@
     </row>
     <row r="402" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A402" s="1">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B402" s="7" t="s">
         <v>858</v>
@@ -14247,7 +14247,7 @@
     </row>
     <row r="403" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A403" s="1">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B403" s="7" t="s">
         <v>909</v>
@@ -14276,7 +14276,7 @@
     </row>
     <row r="404" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A404" s="1">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B404" s="7" t="s">
         <v>444</v>
@@ -14305,7 +14305,7 @@
     </row>
     <row r="405" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A405" s="1">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B405" s="7" t="s">
         <v>473</v>
@@ -14337,7 +14337,7 @@
     </row>
     <row r="406" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A406" s="1">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B406" s="7" t="s">
         <v>479</v>
@@ -14369,7 +14369,7 @@
     </row>
     <row r="407" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A407" s="1">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B407" s="7" t="s">
         <v>428</v>
@@ -14401,7 +14401,7 @@
     </row>
     <row r="408" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A408" s="1">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B408" s="7" t="s">
         <v>424</v>
@@ -14433,7 +14433,7 @@
     </row>
     <row r="409" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A409" s="1">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B409" s="7" t="s">
         <v>426</v>
@@ -14465,7 +14465,7 @@
     </row>
     <row r="410" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A410" s="1">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B410" s="7" t="s">
         <v>430</v>
@@ -14497,7 +14497,7 @@
     </row>
     <row r="411" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A411" s="1">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B411" s="7" t="s">
         <v>434</v>
@@ -14526,7 +14526,7 @@
     </row>
     <row r="412" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A412" s="1">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B412" s="7" t="s">
         <v>510</v>
@@ -14555,7 +14555,7 @@
     </row>
     <row r="413" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A413" s="1">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B413" s="7" t="s">
         <v>417</v>
@@ -14587,7 +14587,7 @@
     </row>
     <row r="414" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A414" s="1">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B414" s="7" t="s">
         <v>420</v>
@@ -14616,7 +14616,7 @@
     </row>
     <row r="415" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A415" s="1">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B415" s="7" t="s">
         <v>468</v>
@@ -14645,7 +14645,7 @@
     </row>
     <row r="416" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A416" s="1">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B416" s="7" t="s">
         <v>440</v>
@@ -14674,7 +14674,7 @@
     </row>
     <row r="417" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A417" s="1">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B417" s="7" t="s">
         <v>450</v>
@@ -14703,7 +14703,7 @@
     </row>
     <row r="418" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A418" s="1">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B418" s="7" t="s">
         <v>459</v>
@@ -14732,7 +14732,7 @@
     </row>
     <row r="419" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A419" s="1">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B419" s="7" t="s">
         <v>436</v>
@@ -14761,7 +14761,7 @@
     </row>
     <row r="420" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A420" s="1">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B420" s="7" t="s">
         <v>453</v>
@@ -14790,7 +14790,7 @@
     </row>
     <row r="421" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A421" s="1">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B421" s="7" t="s">
         <v>438</v>
@@ -14819,7 +14819,7 @@
     </row>
     <row r="422" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A422" s="1">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B422" s="7" t="s">
         <v>515</v>
@@ -14848,7 +14848,7 @@
     </row>
     <row r="423" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A423" s="1">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B423" s="7" t="s">
         <v>518</v>
@@ -14877,7 +14877,7 @@
     </row>
     <row r="424" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A424" s="1">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B424" s="7" t="s">
         <v>461</v>
@@ -14909,7 +14909,7 @@
     </row>
     <row r="425" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A425" s="1">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B425" s="7" t="s">
         <v>513</v>
@@ -14938,7 +14938,7 @@
     </row>
     <row r="426" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A426" s="1">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B426" s="7" t="s">
         <v>485</v>
@@ -14967,7 +14967,7 @@
     </row>
     <row r="427" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A427" s="1">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B427" s="7" t="s">
         <v>481</v>
@@ -14999,7 +14999,7 @@
     </row>
     <row r="428" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A428" s="1">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B428" s="7" t="s">
         <v>455</v>
@@ -15031,7 +15031,7 @@
     </row>
     <row r="429" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A429" s="1">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B429" s="7" t="s">
         <v>154</v>
@@ -15063,7 +15063,7 @@
     </row>
     <row r="430" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A430" s="1">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B430" s="7" t="s">
         <v>517</v>
@@ -15092,7 +15092,7 @@
     </row>
     <row r="431" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A431" s="1">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B431" s="7" t="s">
         <v>520</v>
@@ -15121,7 +15121,7 @@
     </row>
     <row r="432" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A432" s="1">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B432" s="7" t="s">
         <v>463</v>
@@ -15150,7 +15150,7 @@
     </row>
     <row r="433" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A433" s="1">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B433" s="7" t="s">
         <v>471</v>
@@ -15182,7 +15182,7 @@
     </row>
     <row r="434" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A434" s="1">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B434" s="7" t="s">
         <v>457</v>
@@ -15214,7 +15214,7 @@
     </row>
     <row r="435" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A435" s="1">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B435" s="7" t="s">
         <v>465</v>
@@ -15246,7 +15246,7 @@
     </row>
     <row r="436" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A436" s="1">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B436" s="7" t="s">
         <v>446</v>
@@ -15275,7 +15275,7 @@
     </row>
     <row r="437" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A437" s="1">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B437" s="7" t="s">
         <v>448</v>
@@ -15304,7 +15304,7 @@
     </row>
     <row r="438" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A438" s="1">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B438" s="7" t="s">
         <v>477</v>
@@ -15336,7 +15336,7 @@
     </row>
     <row r="439" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A439" s="1">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B439" s="7" t="s">
         <v>491</v>
@@ -15365,7 +15365,7 @@
     </row>
     <row r="440" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A440" s="1">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B440" s="7" t="s">
         <v>489</v>
@@ -15397,7 +15397,7 @@
     </row>
     <row r="441" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A441" s="1">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B441" s="7" t="s">
         <v>483</v>
@@ -15426,7 +15426,7 @@
     </row>
     <row r="442" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A442" s="1">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B442" s="7" t="s">
         <v>487</v>
@@ -15458,7 +15458,7 @@
     </row>
     <row r="443" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A443" s="1">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B443" s="7" t="s">
         <v>523</v>
@@ -15487,7 +15487,7 @@
     </row>
     <row r="444" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A444" s="1">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B444" s="7" t="s">
         <v>522</v>
@@ -15516,7 +15516,7 @@
     </row>
     <row r="445" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A445" s="1">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B445" s="7" t="s">
         <v>499</v>
@@ -15545,7 +15545,7 @@
     </row>
     <row r="446" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A446" s="1">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B446" s="7" t="s">
         <v>503</v>
@@ -15577,7 +15577,7 @@
     </row>
     <row r="447" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A447" s="1">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B447" s="7" t="s">
         <v>501</v>
@@ -15606,7 +15606,7 @@
     </row>
     <row r="448" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A448" s="1">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B448" s="7" t="s">
         <v>525</v>
@@ -15635,7 +15635,7 @@
     </row>
     <row r="449" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A449" s="1">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B449" s="7" t="s">
         <v>524</v>
@@ -15664,7 +15664,7 @@
     </row>
     <row r="450" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A450" s="1">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B450" s="7" t="s">
         <v>508</v>
@@ -15696,7 +15696,7 @@
     </row>
     <row r="451" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A451" s="1">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B451" s="7" t="s">
         <v>833</v>
@@ -15719,7 +15719,7 @@
     </row>
     <row r="452" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A452" s="1">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B452" s="7" t="s">
         <v>835</v>
@@ -15742,7 +15742,7 @@
     </row>
     <row r="453" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A453" s="1">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B453" s="7" t="s">
         <v>837</v>
@@ -15765,7 +15765,7 @@
     </row>
     <row r="454" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A454" s="1">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B454" s="7" t="s">
         <v>839</v>
@@ -15788,7 +15788,7 @@
     </row>
     <row r="455" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A455" s="1">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B455" s="7" t="s">
         <v>843</v>
@@ -15811,7 +15811,7 @@
     </row>
     <row r="456" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A456" s="1">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B456" s="7" t="s">
         <v>845</v>
@@ -15834,7 +15834,7 @@
     </row>
     <row r="457" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A457" s="1">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B457" s="7" t="s">
         <v>847</v>
@@ -15857,7 +15857,7 @@
     </row>
     <row r="458" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A458" s="1">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B458" s="7" t="s">
         <v>852</v>
@@ -15880,7 +15880,7 @@
     </row>
     <row r="459" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A459" s="1">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B459" s="7" t="s">
         <v>854</v>
@@ -15903,7 +15903,7 @@
     </row>
     <row r="460" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A460" s="1">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B460" s="7" t="s">
         <v>862</v>
@@ -15926,7 +15926,7 @@
     </row>
     <row r="461" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A461" s="1">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B461" s="7" t="s">
         <v>864</v>
@@ -15949,7 +15949,7 @@
     </row>
     <row r="462" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A462" s="1">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B462" s="7" t="s">
         <v>866</v>
@@ -15972,7 +15972,7 @@
     </row>
     <row r="463" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A463" s="1">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B463" s="7" t="s">
         <v>868</v>
@@ -15995,7 +15995,7 @@
     </row>
     <row r="464" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A464" s="1">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B464" s="7" t="s">
         <v>870</v>
@@ -16018,7 +16018,7 @@
     </row>
     <row r="465" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A465" s="1">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B465" s="7" t="s">
         <v>872</v>
@@ -16041,7 +16041,7 @@
     </row>
     <row r="466" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A466" s="1">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B466" s="7" t="s">
         <v>874</v>
@@ -16064,7 +16064,7 @@
     </row>
     <row r="467" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A467" s="1">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B467" s="7" t="s">
         <v>880</v>
@@ -16087,7 +16087,7 @@
     </row>
     <row r="468" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A468" s="1">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B468" s="7" t="s">
         <v>884</v>
@@ -16110,7 +16110,7 @@
     </row>
     <row r="469" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A469" s="1">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B469" s="7" t="s">
         <v>911</v>
@@ -16139,7 +16139,7 @@
     </row>
     <row r="470" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A470" s="1">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B470" s="7" t="s">
         <v>913</v>
@@ -16168,7 +16168,7 @@
     </row>
     <row r="471" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A471" s="1">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B471" s="7" t="s">
         <v>915</v>
@@ -16197,7 +16197,7 @@
     </row>
     <row r="472" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A472" s="1">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B472" s="7" t="s">
         <v>919</v>
@@ -16226,7 +16226,7 @@
     </row>
     <row r="473" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A473" s="1">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B473" s="7" t="s">
         <v>920</v>
@@ -16254,8 +16254,8 @@
       </c>
     </row>
     <row r="474" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A474" s="6">
-        <v>473</v>
+      <c r="A474" s="1">
+        <v>472</v>
       </c>
       <c r="B474" s="7" t="s">
         <v>926</v>
@@ -16281,7 +16281,7 @@
     </row>
     <row r="475" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A475" s="1">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B475" s="7" t="s">
         <v>4</v>
@@ -16309,8 +16309,8 @@
       </c>
     </row>
     <row r="476" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A476" s="6">
-        <v>475</v>
+      <c r="A476" s="1">
+        <v>474</v>
       </c>
       <c r="B476" s="7" t="s">
         <v>4</v>
@@ -16339,7 +16339,7 @@
     </row>
     <row r="477" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A477" s="1">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B477" s="7" t="s">
         <v>538</v>
@@ -16361,8 +16361,8 @@
       </c>
     </row>
     <row r="478" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A478" s="6">
-        <v>477</v>
+      <c r="A478" s="1">
+        <v>476</v>
       </c>
       <c r="B478" s="7" t="s">
         <v>422</v>
@@ -16391,7 +16391,7 @@
     </row>
     <row r="479" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A479" s="1">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B479" s="7" t="s">
         <v>432</v>
@@ -16419,8 +16419,8 @@
       </c>
     </row>
     <row r="480" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A480" s="6">
-        <v>479</v>
+      <c r="A480" s="1">
+        <v>478</v>
       </c>
       <c r="B480" s="7" t="s">
         <v>440</v>
@@ -16449,7 +16449,7 @@
     </row>
     <row r="481" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A481" s="1">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B481" s="7" t="s">
         <v>440</v>
@@ -16477,8 +16477,8 @@
       </c>
     </row>
     <row r="482" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A482" s="6">
-        <v>481</v>
+      <c r="A482" s="1">
+        <v>480</v>
       </c>
       <c r="B482" s="7" t="s">
         <v>485</v>

</xml_diff>

<commit_message>
Card changes in version 1.1.0.6024
</commit_message>
<xml_diff>
--- a/card_info.xlsx
+++ b/card_info.xlsx
@@ -2689,9 +2689,6 @@
     <t>Eaglehorn Bow</t>
   </si>
   <si>
-    <t>Whenever a Secret is revealed, gain +1 Durability.</t>
-  </si>
-  <si>
     <t>Gladiator's Longbow</t>
   </si>
   <si>
@@ -2804,6 +2801,9 @@
   </si>
   <si>
     <t>Draw a card. Combo: Draw 2 cards instead.</t>
+  </si>
+  <si>
+    <t>Whenever a friendly Secret is revealed, gain +1 Durability.</t>
   </si>
 </sst>
 </file>
@@ -3208,8 +3208,8 @@
   <dimension ref="A1:J482"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A459" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B482" sqref="B482"/>
+      <pane ySplit="1" topLeftCell="A359" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J373" sqref="J373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3234,7 +3234,7 @@
         <v>528</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>529</v>
@@ -3266,7 +3266,7 @@
         <v>139</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>140</v>
@@ -3294,7 +3294,7 @@
         <v>106</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>103</v>
@@ -3326,7 +3326,7 @@
         <v>84</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>85</v>
@@ -3356,7 +3356,7 @@
         <v>34</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>35</v>
@@ -3386,7 +3386,7 @@
         <v>56</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>57</v>
@@ -3416,7 +3416,7 @@
         <v>108</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>103</v>
@@ -3448,7 +3448,7 @@
         <v>141</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>140</v>
@@ -3478,7 +3478,7 @@
         <v>158</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>140</v>
@@ -3508,7 +3508,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>140</v>
@@ -3538,7 +3538,7 @@
         <v>168</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>140</v>
@@ -3570,7 +3570,7 @@
         <v>171</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>140</v>
@@ -3600,7 +3600,7 @@
         <v>173</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>140</v>
@@ -3630,7 +3630,7 @@
         <v>177</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>140</v>
@@ -3660,7 +3660,7 @@
         <v>147</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>140</v>
@@ -3692,7 +3692,7 @@
         <v>152</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>140</v>
@@ -3722,7 +3722,7 @@
         <v>156</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>140</v>
@@ -3754,7 +3754,7 @@
         <v>160</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>140</v>
@@ -3784,7 +3784,7 @@
         <v>163</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>140</v>
@@ -3816,7 +3816,7 @@
         <v>165</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>140</v>
@@ -3846,7 +3846,7 @@
         <v>143</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>140</v>
@@ -3878,7 +3878,7 @@
         <v>145</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>140</v>
@@ -3908,7 +3908,7 @@
         <v>150</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>140</v>
@@ -3938,7 +3938,7 @@
         <v>153</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>140</v>
@@ -3970,7 +3970,7 @@
         <v>170</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>140</v>
@@ -4002,7 +4002,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>19</v>
@@ -4034,7 +4034,7 @@
         <v>175</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>140</v>
@@ -4066,7 +4066,7 @@
         <v>102</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>103</v>
@@ -4098,7 +4098,7 @@
         <v>167</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>140</v>
@@ -4128,7 +4128,7 @@
         <v>183</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>140</v>
@@ -4158,7 +4158,7 @@
         <v>221</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>140</v>
@@ -4188,7 +4188,7 @@
         <v>109</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>103</v>
@@ -4220,7 +4220,7 @@
         <v>179</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>140</v>
@@ -4250,7 +4250,7 @@
         <v>185</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>140</v>
@@ -4280,7 +4280,7 @@
         <v>199</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>140</v>
@@ -4312,7 +4312,7 @@
         <v>205</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>140</v>
@@ -4342,7 +4342,7 @@
         <v>213</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>140</v>
@@ -4372,7 +4372,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>35</v>
@@ -4402,7 +4402,7 @@
         <v>234</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>140</v>
@@ -4432,7 +4432,7 @@
         <v>236</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>140</v>
@@ -4462,7 +4462,7 @@
         <v>181</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>140</v>
@@ -4492,7 +4492,7 @@
         <v>188</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>140</v>
@@ -4524,7 +4524,7 @@
         <v>231</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>140</v>
@@ -4554,7 +4554,7 @@
         <v>232</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>140</v>
@@ -4584,7 +4584,7 @@
         <v>47</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>48</v>
@@ -4614,7 +4614,7 @@
         <v>193</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>140</v>
@@ -4644,7 +4644,7 @@
         <v>128</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>126</v>
@@ -4674,7 +4674,7 @@
         <v>71</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>72</v>
@@ -4704,7 +4704,7 @@
         <v>195</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>140</v>
@@ -4736,7 +4736,7 @@
         <v>202</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>140</v>
@@ -4766,7 +4766,7 @@
         <v>207</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>140</v>
@@ -4796,7 +4796,7 @@
         <v>217</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>140</v>
@@ -4826,7 +4826,7 @@
         <v>229</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>140</v>
@@ -4856,7 +4856,7 @@
         <v>22</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>19</v>
@@ -4888,7 +4888,7 @@
         <v>125</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>126</v>
@@ -4918,7 +4918,7 @@
         <v>215</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>140</v>
@@ -4948,7 +4948,7 @@
         <v>219</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>140</v>
@@ -4978,7 +4978,7 @@
         <v>190</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>140</v>
@@ -5010,7 +5010,7 @@
         <v>203</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>140</v>
@@ -5042,7 +5042,7 @@
         <v>209</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>140</v>
@@ -5072,7 +5072,7 @@
         <v>223</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>140</v>
@@ -5104,7 +5104,7 @@
         <v>24</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>19</v>
@@ -5136,7 +5136,7 @@
         <v>186</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>140</v>
@@ -5166,7 +5166,7 @@
         <v>191</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>140</v>
@@ -5198,7 +5198,7 @@
         <v>227</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>140</v>
@@ -5228,7 +5228,7 @@
         <v>74</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>72</v>
@@ -5258,7 +5258,7 @@
         <v>197</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>140</v>
@@ -5288,7 +5288,7 @@
         <v>87</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>85</v>
@@ -5320,7 +5320,7 @@
         <v>59</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>57</v>
@@ -5350,7 +5350,7 @@
         <v>211</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>140</v>
@@ -5380,7 +5380,7 @@
         <v>225</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>140</v>
@@ -5410,7 +5410,7 @@
         <v>265</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>140</v>
@@ -5440,7 +5440,7 @@
         <v>270</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>140</v>
@@ -5472,7 +5472,7 @@
         <v>111</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>103</v>
@@ -5504,7 +5504,7 @@
         <v>39</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>35</v>
@@ -5534,7 +5534,7 @@
         <v>50</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>48</v>
@@ -5564,7 +5564,7 @@
         <v>246</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>140</v>
@@ -5594,7 +5594,7 @@
         <v>255</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>140</v>
@@ -5624,7 +5624,7 @@
         <v>268</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>140</v>
@@ -5656,7 +5656,7 @@
         <v>273</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>140</v>
@@ -5686,7 +5686,7 @@
         <v>275</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>140</v>
@@ -5718,7 +5718,7 @@
         <v>279</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>140</v>
@@ -5748,7 +5748,7 @@
         <v>78</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>72</v>
@@ -5778,7 +5778,7 @@
         <v>289</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>140</v>
@@ -5810,7 +5810,7 @@
         <v>294</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>140</v>
@@ -5840,7 +5840,7 @@
         <v>113</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>103</v>
@@ -5872,7 +5872,7 @@
         <v>242</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>140</v>
@@ -5902,7 +5902,7 @@
         <v>244</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>140</v>
@@ -5932,7 +5932,7 @@
         <v>269</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>140</v>
@@ -5964,7 +5964,7 @@
         <v>130</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>126</v>
@@ -5994,7 +5994,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>85</v>
@@ -6024,7 +6024,7 @@
         <v>286</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>140</v>
@@ -6054,7 +6054,7 @@
         <v>250</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>140</v>
@@ -6086,7 +6086,7 @@
         <v>257</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>140</v>
@@ -6118,7 +6118,7 @@
         <v>259</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>140</v>
@@ -6148,7 +6148,7 @@
         <v>261</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>140</v>
@@ -6178,7 +6178,7 @@
         <v>283</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>140</v>
@@ -6208,7 +6208,7 @@
         <v>291</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>140</v>
@@ -6238,7 +6238,7 @@
         <v>293</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>140</v>
@@ -6268,7 +6268,7 @@
         <v>132</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>126</v>
@@ -6298,7 +6298,7 @@
         <v>272</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>140</v>
@@ -6326,7 +6326,7 @@
         <v>263</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>140</v>
@@ -6356,7 +6356,7 @@
         <v>248</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>140</v>
@@ -6388,7 +6388,7 @@
         <v>76</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>72</v>
@@ -6418,7 +6418,7 @@
         <v>267</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>140</v>
@@ -6448,7 +6448,7 @@
         <v>277</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>140</v>
@@ -6478,7 +6478,7 @@
         <v>281</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>140</v>
@@ -6508,7 +6508,7 @@
         <v>252</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>140</v>
@@ -6538,7 +6538,7 @@
         <v>253</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>140</v>
@@ -6568,7 +6568,7 @@
         <v>288</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>140</v>
@@ -6600,7 +6600,7 @@
         <v>285</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>140</v>
@@ -6630,7 +6630,7 @@
         <v>296</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>140</v>
@@ -6660,7 +6660,7 @@
         <v>238</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>140</v>
@@ -6690,7 +6690,7 @@
         <v>240</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>140</v>
@@ -6720,7 +6720,7 @@
         <v>90</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>85</v>
@@ -6752,7 +6752,7 @@
         <v>115</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>103</v>
@@ -6784,7 +6784,7 @@
         <v>297</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>140</v>
@@ -6814,7 +6814,7 @@
         <v>300</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>140</v>
@@ -6842,7 +6842,7 @@
         <v>43</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>35</v>
@@ -6872,7 +6872,7 @@
         <v>303</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>140</v>
@@ -6902,7 +6902,7 @@
         <v>80</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>72</v>
@@ -6932,7 +6932,7 @@
         <v>315</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>140</v>
@@ -6962,7 +6962,7 @@
         <v>61</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>57</v>
@@ -6992,7 +6992,7 @@
         <v>318</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>140</v>
@@ -7022,7 +7022,7 @@
         <v>324</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>140</v>
@@ -7052,7 +7052,7 @@
         <v>314</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>140</v>
@@ -7082,7 +7082,7 @@
         <v>311</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>140</v>
@@ -7112,7 +7112,7 @@
         <v>26</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>19</v>
@@ -7142,7 +7142,7 @@
         <v>136</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>126</v>
@@ -7172,7 +7172,7 @@
         <v>320</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>140</v>
@@ -7202,7 +7202,7 @@
         <v>298</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>140</v>
@@ -7232,7 +7232,7 @@
         <v>321</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>140</v>
@@ -7262,7 +7262,7 @@
         <v>134</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>126</v>
@@ -7292,7 +7292,7 @@
         <v>308</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>140</v>
@@ -7324,7 +7324,7 @@
         <v>41</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>35</v>
@@ -7354,7 +7354,7 @@
         <v>319</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>140</v>
@@ -7384,7 +7384,7 @@
         <v>94</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>85</v>
@@ -7414,7 +7414,7 @@
         <v>301</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>140</v>
@@ -7444,7 +7444,7 @@
         <v>306</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>140</v>
@@ -7474,7 +7474,7 @@
         <v>310</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>140</v>
@@ -7504,7 +7504,7 @@
         <v>0</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>1</v>
@@ -7534,7 +7534,7 @@
         <v>316</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>140</v>
@@ -7566,7 +7566,7 @@
         <v>313</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>140</v>
@@ -7596,7 +7596,7 @@
         <v>304</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>140</v>
@@ -7626,7 +7626,7 @@
         <v>322</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>140</v>
@@ -7658,7 +7658,7 @@
         <v>63</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>57</v>
@@ -7688,7 +7688,7 @@
         <v>117</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>103</v>
@@ -7718,7 +7718,7 @@
         <v>96</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>85</v>
@@ -7748,7 +7748,7 @@
         <v>359</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>140</v>
@@ -7778,7 +7778,7 @@
         <v>119</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>103</v>
@@ -7810,7 +7810,7 @@
         <v>335</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>140</v>
@@ -7840,7 +7840,7 @@
         <v>358</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>140</v>
@@ -7872,7 +7872,7 @@
         <v>352</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>140</v>
@@ -7902,7 +7902,7 @@
         <v>330</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>140</v>
@@ -7932,7 +7932,7 @@
         <v>331</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>140</v>
@@ -7964,7 +7964,7 @@
         <v>346</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>140</v>
@@ -7994,7 +7994,7 @@
         <v>333</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>140</v>
@@ -8024,7 +8024,7 @@
         <v>339</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>140</v>
@@ -8054,7 +8054,7 @@
         <v>326</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>140</v>
@@ -8084,7 +8084,7 @@
         <v>328</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>140</v>
@@ -8116,7 +8116,7 @@
         <v>4</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>1</v>
@@ -8146,7 +8146,7 @@
         <v>340</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>140</v>
@@ -8176,7 +8176,7 @@
         <v>342</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>140</v>
@@ -8206,7 +8206,7 @@
         <v>348</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>140</v>
@@ -8236,7 +8236,7 @@
         <v>350</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>140</v>
@@ -8266,7 +8266,7 @@
         <v>354</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>140</v>
@@ -8298,7 +8298,7 @@
         <v>344</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>140</v>
@@ -8328,7 +8328,7 @@
         <v>28</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>19</v>
@@ -8360,7 +8360,7 @@
         <v>337</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>140</v>
@@ -8390,7 +8390,7 @@
         <v>356</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>140</v>
@@ -8420,7 +8420,7 @@
         <v>383</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>140</v>
@@ -8452,7 +8452,7 @@
         <v>364</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>140</v>
@@ -8480,7 +8480,7 @@
         <v>121</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>103</v>
@@ -8512,7 +8512,7 @@
         <v>369</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>140</v>
@@ -8542,7 +8542,7 @@
         <v>67</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>57</v>
@@ -8572,7 +8572,7 @@
         <v>373</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>140</v>
@@ -8604,7 +8604,7 @@
         <v>98</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>85</v>
@@ -8634,7 +8634,7 @@
         <v>375</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>140</v>
@@ -8664,7 +8664,7 @@
         <v>30</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>19</v>
@@ -8696,7 +8696,7 @@
         <v>361</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>140</v>
@@ -8726,7 +8726,7 @@
         <v>367</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>140</v>
@@ -8756,7 +8756,7 @@
         <v>381</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>140</v>
@@ -8786,7 +8786,7 @@
         <v>376</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>140</v>
@@ -8816,7 +8816,7 @@
         <v>65</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>57</v>
@@ -8846,7 +8846,7 @@
         <v>365</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>140</v>
@@ -8876,7 +8876,7 @@
         <v>379</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>140</v>
@@ -8906,7 +8906,7 @@
         <v>385</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>140</v>
@@ -8936,7 +8936,7 @@
         <v>387</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>140</v>
@@ -8966,7 +8966,7 @@
         <v>371</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>140</v>
@@ -8996,7 +8996,7 @@
         <v>82</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>72</v>
@@ -9026,7 +9026,7 @@
         <v>378</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>140</v>
@@ -9056,7 +9056,7 @@
         <v>362</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>140</v>
@@ -9086,7 +9086,7 @@
         <v>69</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>57</v>
@@ -9116,7 +9116,7 @@
         <v>394</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>140</v>
@@ -9144,7 +9144,7 @@
         <v>390</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>140</v>
@@ -9174,7 +9174,7 @@
         <v>392</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>140</v>
@@ -9204,7 +9204,7 @@
         <v>388</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>140</v>
@@ -9234,7 +9234,7 @@
         <v>391</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>140</v>
@@ -9264,7 +9264,7 @@
         <v>45</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>35</v>
@@ -9294,7 +9294,7 @@
         <v>52</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>48</v>
@@ -9324,7 +9324,7 @@
         <v>7</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>1</v>
@@ -9354,7 +9354,7 @@
         <v>10</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>1</v>
@@ -9384,7 +9384,7 @@
         <v>12</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D203" s="2" t="s">
         <v>1</v>
@@ -9414,7 +9414,7 @@
         <v>397</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D204" s="2" t="s">
         <v>140</v>
@@ -9444,7 +9444,7 @@
         <v>395</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D205" s="2" t="s">
         <v>140</v>
@@ -9474,7 +9474,7 @@
         <v>54</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D206" s="2" t="s">
         <v>48</v>
@@ -9504,7 +9504,7 @@
         <v>137</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>126</v>
@@ -9534,7 +9534,7 @@
         <v>100</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D208" s="2" t="s">
         <v>85</v>
@@ -9564,7 +9564,7 @@
         <v>399</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D209" s="2" t="s">
         <v>140</v>
@@ -9596,7 +9596,7 @@
         <v>32</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D210" s="2" t="s">
         <v>19</v>
@@ -9628,7 +9628,7 @@
         <v>403</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D211" s="2" t="s">
         <v>140</v>
@@ -9660,7 +9660,7 @@
         <v>405</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D212" s="2" t="s">
         <v>140</v>
@@ -9692,7 +9692,7 @@
         <v>401</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D213" s="2" t="s">
         <v>140</v>
@@ -9724,7 +9724,7 @@
         <v>407</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D214" s="2" t="s">
         <v>140</v>
@@ -9756,7 +9756,7 @@
         <v>123</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D215" s="2" t="s">
         <v>103</v>
@@ -9788,7 +9788,7 @@
         <v>15</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D216" s="2" t="s">
         <v>1</v>
@@ -9818,7 +9818,7 @@
         <v>409</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D217" s="2" t="s">
         <v>140</v>
@@ -9850,7 +9850,7 @@
         <v>411</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D218" s="2" t="s">
         <v>140</v>
@@ -9880,7 +9880,7 @@
         <v>413</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D219" s="2" t="s">
         <v>140</v>
@@ -9910,7 +9910,7 @@
         <v>415</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D220" s="2" t="s">
         <v>140</v>
@@ -9940,7 +9940,7 @@
         <v>536</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D221" s="2" t="s">
         <v>1</v>
@@ -9963,7 +9963,7 @@
         <v>538</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D222" s="2" t="s">
         <v>1</v>
@@ -9986,7 +9986,7 @@
         <v>540</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D223" s="2" t="s">
         <v>1</v>
@@ -10009,7 +10009,7 @@
         <v>542</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D224" s="2" t="s">
         <v>1</v>
@@ -10032,7 +10032,7 @@
         <v>544</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D225" s="2" t="s">
         <v>1</v>
@@ -10055,7 +10055,7 @@
         <v>546</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D226" s="2" t="s">
         <v>1</v>
@@ -10078,7 +10078,7 @@
         <v>548</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D227" s="2" t="s">
         <v>1</v>
@@ -10101,7 +10101,7 @@
         <v>550</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D228" s="2" t="s">
         <v>1</v>
@@ -10124,7 +10124,7 @@
         <v>552</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D229" s="2" t="s">
         <v>1</v>
@@ -10147,7 +10147,7 @@
         <v>554</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D230" s="2" t="s">
         <v>1</v>
@@ -10170,7 +10170,7 @@
         <v>556</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D231" s="2" t="s">
         <v>1</v>
@@ -10193,7 +10193,7 @@
         <v>558</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D232" s="2" t="s">
         <v>1</v>
@@ -10216,7 +10216,7 @@
         <v>560</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D233" s="2" t="s">
         <v>1</v>
@@ -10239,7 +10239,7 @@
         <v>562</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D234" s="2" t="s">
         <v>1</v>
@@ -10262,7 +10262,7 @@
         <v>564</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D235" s="2" t="s">
         <v>1</v>
@@ -10285,7 +10285,7 @@
         <v>566</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D236" s="2" t="s">
         <v>1</v>
@@ -10308,7 +10308,7 @@
         <v>568</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D237" s="2" t="s">
         <v>1</v>
@@ -10331,7 +10331,7 @@
         <v>570</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D238" s="2" t="s">
         <v>1</v>
@@ -10354,7 +10354,7 @@
         <v>572</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D239" s="2" t="s">
         <v>1</v>
@@ -10377,7 +10377,7 @@
         <v>574</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D240" s="2" t="s">
         <v>19</v>
@@ -10400,7 +10400,7 @@
         <v>576</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D241" s="2" t="s">
         <v>19</v>
@@ -10423,7 +10423,7 @@
         <v>578</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D242" s="2" t="s">
         <v>19</v>
@@ -10446,7 +10446,7 @@
         <v>580</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D243" s="2" t="s">
         <v>19</v>
@@ -10469,7 +10469,7 @@
         <v>582</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D244" s="2" t="s">
         <v>19</v>
@@ -10492,7 +10492,7 @@
         <v>584</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D245" s="2" t="s">
         <v>19</v>
@@ -10515,7 +10515,7 @@
         <v>586</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D246" s="2" t="s">
         <v>19</v>
@@ -10538,7 +10538,7 @@
         <v>588</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D247" s="2" t="s">
         <v>19</v>
@@ -10561,7 +10561,7 @@
         <v>590</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D248" s="2" t="s">
         <v>19</v>
@@ -10584,7 +10584,7 @@
         <v>592</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D249" s="2" t="s">
         <v>19</v>
@@ -10607,7 +10607,7 @@
         <v>594</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D250" s="2" t="s">
         <v>19</v>
@@ -10630,7 +10630,7 @@
         <v>596</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D251" s="2" t="s">
         <v>19</v>
@@ -10653,7 +10653,7 @@
         <v>598</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D252" s="2" t="s">
         <v>19</v>
@@ -10676,7 +10676,7 @@
         <v>600</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D253" s="2" t="s">
         <v>19</v>
@@ -10699,7 +10699,7 @@
         <v>602</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D254" s="2" t="s">
         <v>19</v>
@@ -10722,7 +10722,7 @@
         <v>604</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D255" s="2" t="s">
         <v>19</v>
@@ -10745,7 +10745,7 @@
         <v>606</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D256" s="2" t="s">
         <v>35</v>
@@ -10768,7 +10768,7 @@
         <v>608</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D257" s="2" t="s">
         <v>35</v>
@@ -10791,7 +10791,7 @@
         <v>422</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D258" s="2" t="s">
         <v>35</v>
@@ -10814,7 +10814,7 @@
         <v>611</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D259" s="2" t="s">
         <v>35</v>
@@ -10837,7 +10837,7 @@
         <v>613</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D260" s="2" t="s">
         <v>35</v>
@@ -10860,7 +10860,7 @@
         <v>615</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D261" s="2" t="s">
         <v>35</v>
@@ -10883,7 +10883,7 @@
         <v>617</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D262" s="2" t="s">
         <v>35</v>
@@ -10906,7 +10906,7 @@
         <v>619</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D263" s="2" t="s">
         <v>35</v>
@@ -10929,7 +10929,7 @@
         <v>621</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D264" s="2" t="s">
         <v>35</v>
@@ -10952,7 +10952,7 @@
         <v>623</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D265" s="2" t="s">
         <v>35</v>
@@ -10975,7 +10975,7 @@
         <v>625</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D266" s="2" t="s">
         <v>35</v>
@@ -10998,7 +10998,7 @@
         <v>432</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D267" s="2" t="s">
         <v>35</v>
@@ -11021,7 +11021,7 @@
         <v>628</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D268" s="2" t="s">
         <v>35</v>
@@ -11044,7 +11044,7 @@
         <v>630</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D269" s="2" t="s">
         <v>35</v>
@@ -11067,7 +11067,7 @@
         <v>632</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D270" s="2" t="s">
         <v>35</v>
@@ -11090,7 +11090,7 @@
         <v>634</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D271" s="2" t="s">
         <v>35</v>
@@ -11113,7 +11113,7 @@
         <v>636</v>
       </c>
       <c r="C272" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D272" s="2" t="s">
         <v>35</v>
@@ -11136,7 +11136,7 @@
         <v>638</v>
       </c>
       <c r="C273" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D273" s="2" t="s">
         <v>35</v>
@@ -11159,7 +11159,7 @@
         <v>640</v>
       </c>
       <c r="C274" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D274" s="2" t="s">
         <v>35</v>
@@ -11182,7 +11182,7 @@
         <v>642</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D275" s="2" t="s">
         <v>48</v>
@@ -11205,7 +11205,7 @@
         <v>644</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D276" s="2" t="s">
         <v>48</v>
@@ -11228,7 +11228,7 @@
         <v>646</v>
       </c>
       <c r="C277" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D277" s="2" t="s">
         <v>48</v>
@@ -11251,7 +11251,7 @@
         <v>648</v>
       </c>
       <c r="C278" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D278" s="2" t="s">
         <v>48</v>
@@ -11274,7 +11274,7 @@
         <v>650</v>
       </c>
       <c r="C279" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D279" s="2" t="s">
         <v>48</v>
@@ -11297,7 +11297,7 @@
         <v>652</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D280" s="2" t="s">
         <v>48</v>
@@ -11320,7 +11320,7 @@
         <v>654</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D281" s="2" t="s">
         <v>48</v>
@@ -11343,7 +11343,7 @@
         <v>656</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D282" s="2" t="s">
         <v>48</v>
@@ -11366,7 +11366,7 @@
         <v>658</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D283" s="2" t="s">
         <v>48</v>
@@ -11389,7 +11389,7 @@
         <v>660</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D284" s="2" t="s">
         <v>48</v>
@@ -11412,7 +11412,7 @@
         <v>662</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D285" s="2" t="s">
         <v>48</v>
@@ -11435,7 +11435,7 @@
         <v>664</v>
       </c>
       <c r="C286" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D286" s="2" t="s">
         <v>48</v>
@@ -11458,7 +11458,7 @@
         <v>666</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D287" s="2" t="s">
         <v>48</v>
@@ -11481,7 +11481,7 @@
         <v>668</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D288" s="2" t="s">
         <v>48</v>
@@ -11504,7 +11504,7 @@
         <v>670</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D289" s="2" t="s">
         <v>48</v>
@@ -11527,7 +11527,7 @@
         <v>672</v>
       </c>
       <c r="C290" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D290" s="2" t="s">
         <v>48</v>
@@ -11550,7 +11550,7 @@
         <v>674</v>
       </c>
       <c r="C291" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D291" s="2" t="s">
         <v>48</v>
@@ -11573,7 +11573,7 @@
         <v>676</v>
       </c>
       <c r="C292" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D292" s="2" t="s">
         <v>48</v>
@@ -11596,7 +11596,7 @@
         <v>678</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D293" s="2" t="s">
         <v>57</v>
@@ -11619,7 +11619,7 @@
         <v>680</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D294" s="2" t="s">
         <v>57</v>
@@ -11642,7 +11642,7 @@
         <v>682</v>
       </c>
       <c r="C295" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D295" s="2" t="s">
         <v>57</v>
@@ -11665,7 +11665,7 @@
         <v>683</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D296" s="2" t="s">
         <v>57</v>
@@ -11688,7 +11688,7 @@
         <v>685</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D297" s="2" t="s">
         <v>57</v>
@@ -11711,7 +11711,7 @@
         <v>687</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D298" s="2" t="s">
         <v>57</v>
@@ -11734,7 +11734,7 @@
         <v>689</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D299" s="2" t="s">
         <v>57</v>
@@ -11757,7 +11757,7 @@
         <v>691</v>
       </c>
       <c r="C300" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D300" s="2" t="s">
         <v>57</v>
@@ -11780,7 +11780,7 @@
         <v>693</v>
       </c>
       <c r="C301" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D301" s="2" t="s">
         <v>57</v>
@@ -11803,7 +11803,7 @@
         <v>695</v>
       </c>
       <c r="C302" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D302" s="2" t="s">
         <v>57</v>
@@ -11826,7 +11826,7 @@
         <v>697</v>
       </c>
       <c r="C303" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D303" s="2" t="s">
         <v>57</v>
@@ -11849,7 +11849,7 @@
         <v>699</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D304" s="2" t="s">
         <v>57</v>
@@ -11872,7 +11872,7 @@
         <v>701</v>
       </c>
       <c r="C305" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D305" s="2" t="s">
         <v>57</v>
@@ -11895,7 +11895,7 @@
         <v>703</v>
       </c>
       <c r="C306" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D306" s="2" t="s">
         <v>57</v>
@@ -11918,7 +11918,7 @@
         <v>705</v>
       </c>
       <c r="C307" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D307" s="2" t="s">
         <v>57</v>
@@ -11941,7 +11941,7 @@
         <v>707</v>
       </c>
       <c r="C308" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D308" s="2" t="s">
         <v>57</v>
@@ -11964,7 +11964,7 @@
         <v>709</v>
       </c>
       <c r="C309" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D309" s="2" t="s">
         <v>57</v>
@@ -11987,7 +11987,7 @@
         <v>711</v>
       </c>
       <c r="C310" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D310" s="2" t="s">
         <v>57</v>
@@ -12010,7 +12010,7 @@
         <v>713</v>
       </c>
       <c r="C311" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D311" s="2" t="s">
         <v>72</v>
@@ -12033,7 +12033,7 @@
         <v>715</v>
       </c>
       <c r="C312" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D312" s="2" t="s">
         <v>72</v>
@@ -12056,7 +12056,7 @@
         <v>717</v>
       </c>
       <c r="C313" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D313" s="2" t="s">
         <v>72</v>
@@ -12079,7 +12079,7 @@
         <v>719</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D314" s="2" t="s">
         <v>72</v>
@@ -12102,7 +12102,7 @@
         <v>721</v>
       </c>
       <c r="C315" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D315" s="2" t="s">
         <v>72</v>
@@ -12125,7 +12125,7 @@
         <v>723</v>
       </c>
       <c r="C316" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D316" s="2" t="s">
         <v>72</v>
@@ -12148,7 +12148,7 @@
         <v>725</v>
       </c>
       <c r="C317" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D317" s="2" t="s">
         <v>72</v>
@@ -12171,7 +12171,7 @@
         <v>727</v>
       </c>
       <c r="C318" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D318" s="2" t="s">
         <v>72</v>
@@ -12194,7 +12194,7 @@
         <v>729</v>
       </c>
       <c r="C319" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D319" s="2" t="s">
         <v>72</v>
@@ -12217,7 +12217,7 @@
         <v>731</v>
       </c>
       <c r="C320" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D320" s="2" t="s">
         <v>72</v>
@@ -12240,7 +12240,7 @@
         <v>733</v>
       </c>
       <c r="C321" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D321" s="2" t="s">
         <v>72</v>
@@ -12263,7 +12263,7 @@
         <v>735</v>
       </c>
       <c r="C322" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D322" s="2" t="s">
         <v>72</v>
@@ -12286,7 +12286,7 @@
         <v>737</v>
       </c>
       <c r="C323" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D323" s="2" t="s">
         <v>72</v>
@@ -12309,7 +12309,7 @@
         <v>739</v>
       </c>
       <c r="C324" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D324" s="2" t="s">
         <v>72</v>
@@ -12332,7 +12332,7 @@
         <v>741</v>
       </c>
       <c r="C325" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D325" s="2" t="s">
         <v>72</v>
@@ -12355,7 +12355,7 @@
         <v>743</v>
       </c>
       <c r="C326" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D326" s="2" t="s">
         <v>72</v>
@@ -12378,7 +12378,7 @@
         <v>745</v>
       </c>
       <c r="C327" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D327" s="2" t="s">
         <v>72</v>
@@ -12401,7 +12401,7 @@
         <v>747</v>
       </c>
       <c r="C328" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D328" s="2" t="s">
         <v>85</v>
@@ -12424,7 +12424,7 @@
         <v>749</v>
       </c>
       <c r="C329" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D329" s="2" t="s">
         <v>85</v>
@@ -12447,7 +12447,7 @@
         <v>751</v>
       </c>
       <c r="C330" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D330" s="2" t="s">
         <v>85</v>
@@ -12470,7 +12470,7 @@
         <v>753</v>
       </c>
       <c r="C331" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D331" s="2" t="s">
         <v>85</v>
@@ -12493,7 +12493,7 @@
         <v>755</v>
       </c>
       <c r="C332" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D332" s="2" t="s">
         <v>85</v>
@@ -12516,7 +12516,7 @@
         <v>757</v>
       </c>
       <c r="C333" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D333" s="2" t="s">
         <v>85</v>
@@ -12539,7 +12539,7 @@
         <v>759</v>
       </c>
       <c r="C334" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D334" s="2" t="s">
         <v>85</v>
@@ -12562,7 +12562,7 @@
         <v>761</v>
       </c>
       <c r="C335" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D335" s="2" t="s">
         <v>85</v>
@@ -12585,7 +12585,7 @@
         <v>176</v>
       </c>
       <c r="C336" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D336" s="2" t="s">
         <v>85</v>
@@ -12608,7 +12608,7 @@
         <v>764</v>
       </c>
       <c r="C337" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D337" s="2" t="s">
         <v>85</v>
@@ -12631,7 +12631,7 @@
         <v>766</v>
       </c>
       <c r="C338" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D338" s="2" t="s">
         <v>85</v>
@@ -12654,7 +12654,7 @@
         <v>768</v>
       </c>
       <c r="C339" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D339" s="2" t="s">
         <v>85</v>
@@ -12677,7 +12677,7 @@
         <v>770</v>
       </c>
       <c r="C340" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D340" s="2" t="s">
         <v>85</v>
@@ -12700,7 +12700,7 @@
         <v>772</v>
       </c>
       <c r="C341" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D341" s="2" t="s">
         <v>85</v>
@@ -12723,7 +12723,7 @@
         <v>774</v>
       </c>
       <c r="C342" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D342" s="2" t="s">
         <v>85</v>
@@ -12746,7 +12746,7 @@
         <v>776</v>
       </c>
       <c r="C343" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D343" s="2" t="s">
         <v>103</v>
@@ -12769,7 +12769,7 @@
         <v>778</v>
       </c>
       <c r="C344" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D344" s="2" t="s">
         <v>103</v>
@@ -12792,7 +12792,7 @@
         <v>780</v>
       </c>
       <c r="C345" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D345" s="2" t="s">
         <v>103</v>
@@ -12815,7 +12815,7 @@
         <v>782</v>
       </c>
       <c r="C346" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D346" s="2" t="s">
         <v>103</v>
@@ -12838,7 +12838,7 @@
         <v>784</v>
       </c>
       <c r="C347" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D347" s="2" t="s">
         <v>103</v>
@@ -12861,7 +12861,7 @@
         <v>786</v>
       </c>
       <c r="C348" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D348" s="2" t="s">
         <v>103</v>
@@ -12884,7 +12884,7 @@
         <v>788</v>
       </c>
       <c r="C349" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D349" s="2" t="s">
         <v>103</v>
@@ -12907,7 +12907,7 @@
         <v>790</v>
       </c>
       <c r="C350" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D350" s="2" t="s">
         <v>103</v>
@@ -12930,7 +12930,7 @@
         <v>792</v>
       </c>
       <c r="C351" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D351" s="2" t="s">
         <v>103</v>
@@ -12953,7 +12953,7 @@
         <v>794</v>
       </c>
       <c r="C352" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D352" s="2" t="s">
         <v>103</v>
@@ -12976,7 +12976,7 @@
         <v>796</v>
       </c>
       <c r="C353" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D353" s="2" t="s">
         <v>103</v>
@@ -12999,7 +12999,7 @@
         <v>798</v>
       </c>
       <c r="C354" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D354" s="2" t="s">
         <v>103</v>
@@ -13022,7 +13022,7 @@
         <v>800</v>
       </c>
       <c r="C355" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D355" s="2" t="s">
         <v>103</v>
@@ -13045,7 +13045,7 @@
         <v>802</v>
       </c>
       <c r="C356" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D356" s="2" t="s">
         <v>103</v>
@@ -13068,7 +13068,7 @@
         <v>804</v>
       </c>
       <c r="C357" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D357" s="2" t="s">
         <v>126</v>
@@ -13091,7 +13091,7 @@
         <v>806</v>
       </c>
       <c r="C358" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D358" s="2" t="s">
         <v>126</v>
@@ -13114,7 +13114,7 @@
         <v>808</v>
       </c>
       <c r="C359" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D359" s="2" t="s">
         <v>126</v>
@@ -13137,7 +13137,7 @@
         <v>810</v>
       </c>
       <c r="C360" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D360" s="2" t="s">
         <v>126</v>
@@ -13160,7 +13160,7 @@
         <v>812</v>
       </c>
       <c r="C361" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D361" s="2" t="s">
         <v>126</v>
@@ -13183,7 +13183,7 @@
         <v>814</v>
       </c>
       <c r="C362" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D362" s="2" t="s">
         <v>126</v>
@@ -13206,7 +13206,7 @@
         <v>816</v>
       </c>
       <c r="C363" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D363" s="2" t="s">
         <v>126</v>
@@ -13229,7 +13229,7 @@
         <v>818</v>
       </c>
       <c r="C364" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D364" s="2" t="s">
         <v>126</v>
@@ -13252,7 +13252,7 @@
         <v>820</v>
       </c>
       <c r="C365" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D365" s="2" t="s">
         <v>126</v>
@@ -13275,7 +13275,7 @@
         <v>822</v>
       </c>
       <c r="C366" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D366" s="2" t="s">
         <v>126</v>
@@ -13298,7 +13298,7 @@
         <v>824</v>
       </c>
       <c r="C367" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D367" s="2" t="s">
         <v>126</v>
@@ -13321,7 +13321,7 @@
         <v>33</v>
       </c>
       <c r="C368" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D368" s="2" t="s">
         <v>126</v>
@@ -13344,7 +13344,7 @@
         <v>827</v>
       </c>
       <c r="C369" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D369" s="2" t="s">
         <v>126</v>
@@ -13367,7 +13367,7 @@
         <v>829</v>
       </c>
       <c r="C370" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D370" s="2" t="s">
         <v>126</v>
@@ -13390,7 +13390,7 @@
         <v>831</v>
       </c>
       <c r="C371" s="2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D371" s="2" t="s">
         <v>126</v>
@@ -13413,7 +13413,7 @@
         <v>889</v>
       </c>
       <c r="C372" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D372" s="2" t="s">
         <v>19</v>
@@ -13431,7 +13431,7 @@
         <v>2</v>
       </c>
       <c r="J372" s="2" t="s">
-        <v>890</v>
+        <v>928</v>
       </c>
     </row>
     <row r="373" spans="1:10" x14ac:dyDescent="0.25">
@@ -13439,10 +13439,10 @@
         <v>371</v>
       </c>
       <c r="B373" s="2" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C373" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D373" s="2" t="s">
         <v>19</v>
@@ -13460,7 +13460,7 @@
         <v>2</v>
       </c>
       <c r="J373" s="2" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="374" spans="1:10" x14ac:dyDescent="0.25">
@@ -13468,10 +13468,10 @@
         <v>372</v>
       </c>
       <c r="B374" s="2" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="C374" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D374" s="2" t="s">
         <v>48</v>
@@ -13495,10 +13495,10 @@
         <v>373</v>
       </c>
       <c r="B375" s="2" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="C375" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D375" s="2" t="s">
         <v>48</v>
@@ -13516,7 +13516,7 @@
         <v>5</v>
       </c>
       <c r="J375" s="2" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="376" spans="1:10" x14ac:dyDescent="0.25">
@@ -13524,10 +13524,10 @@
         <v>374</v>
       </c>
       <c r="B376" s="2" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C376" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D376" s="2" t="s">
         <v>48</v>
@@ -13545,7 +13545,7 @@
         <v>2</v>
       </c>
       <c r="J376" s="2" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="377" spans="1:10" x14ac:dyDescent="0.25">
@@ -13553,10 +13553,10 @@
         <v>375</v>
       </c>
       <c r="B377" s="2" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="C377" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D377" s="2" t="s">
         <v>72</v>
@@ -13574,7 +13574,7 @@
         <v>2</v>
       </c>
       <c r="J377" s="2" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="378" spans="1:10" x14ac:dyDescent="0.25">
@@ -13582,10 +13582,10 @@
         <v>376</v>
       </c>
       <c r="B378" s="2" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C378" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D378" s="2" t="s">
         <v>72</v>
@@ -13609,10 +13609,10 @@
         <v>377</v>
       </c>
       <c r="B379" s="2" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C379" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D379" s="2" t="s">
         <v>85</v>
@@ -13630,7 +13630,7 @@
         <v>3</v>
       </c>
       <c r="J379" s="2" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="380" spans="1:10" x14ac:dyDescent="0.25">
@@ -13638,10 +13638,10 @@
         <v>378</v>
       </c>
       <c r="B380" s="2" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C380" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D380" s="2" t="s">
         <v>85</v>
@@ -13659,7 +13659,7 @@
         <v>8</v>
       </c>
       <c r="J380" s="2" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="381" spans="1:10" x14ac:dyDescent="0.25">
@@ -13667,10 +13667,10 @@
         <v>379</v>
       </c>
       <c r="B381" s="2" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C381" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D381" s="2" t="s">
         <v>126</v>
@@ -13694,10 +13694,10 @@
         <v>380</v>
       </c>
       <c r="B382" s="2" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C382" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D382" s="2" t="s">
         <v>126</v>
@@ -13721,10 +13721,10 @@
         <v>381</v>
       </c>
       <c r="B383" s="2" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C383" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D383" s="2" t="s">
         <v>126</v>
@@ -13742,7 +13742,7 @@
         <v>1</v>
       </c>
       <c r="J383" s="2" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="384" spans="1:10" x14ac:dyDescent="0.25">
@@ -13750,13 +13750,13 @@
         <v>382</v>
       </c>
       <c r="B384" s="7" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="C384" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D384" s="7" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F384" s="7" t="s">
         <v>8</v>
@@ -13765,7 +13765,7 @@
         <v>1</v>
       </c>
       <c r="J384" s="7" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="385" spans="1:10" x14ac:dyDescent="0.25">
@@ -13776,7 +13776,7 @@
         <v>886</v>
       </c>
       <c r="C385" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D385" s="7" t="s">
         <v>511</v>
@@ -13799,7 +13799,7 @@
         <v>888</v>
       </c>
       <c r="C386" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D386" s="7" t="s">
         <v>511</v>
@@ -13822,7 +13822,7 @@
         <v>493</v>
       </c>
       <c r="C387" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D387" s="7" t="s">
         <v>418</v>
@@ -13854,7 +13854,7 @@
         <v>495</v>
       </c>
       <c r="C388" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D388" s="7" t="s">
         <v>418</v>
@@ -13886,7 +13886,7 @@
         <v>497</v>
       </c>
       <c r="C389" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D389" s="7" t="s">
         <v>418</v>
@@ -13918,7 +13918,7 @@
         <v>507</v>
       </c>
       <c r="C390" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D390" s="7" t="s">
         <v>418</v>
@@ -13950,7 +13950,7 @@
         <v>876</v>
       </c>
       <c r="C391" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D391" s="7" t="s">
         <v>511</v>
@@ -13973,7 +13973,7 @@
         <v>860</v>
       </c>
       <c r="C392" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D392" s="7" t="s">
         <v>418</v>
@@ -13996,7 +13996,7 @@
         <v>882</v>
       </c>
       <c r="C393" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D393" s="7" t="s">
         <v>511</v>
@@ -14016,10 +14016,10 @@
         <v>392</v>
       </c>
       <c r="B394" s="7" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C394" s="7" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D394" s="7" t="s">
         <v>418</v>
@@ -14037,7 +14037,7 @@
         <v>3</v>
       </c>
       <c r="J394" s="7" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="395" spans="1:10" x14ac:dyDescent="0.25">
@@ -14048,7 +14048,7 @@
         <v>526</v>
       </c>
       <c r="C395" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D395" s="7" t="s">
         <v>511</v>
@@ -14077,7 +14077,7 @@
         <v>475</v>
       </c>
       <c r="C396" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D396" s="7" t="s">
         <v>418</v>
@@ -14109,7 +14109,7 @@
         <v>442</v>
       </c>
       <c r="C397" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D397" s="7" t="s">
         <v>418</v>
@@ -14138,7 +14138,7 @@
         <v>878</v>
       </c>
       <c r="C398" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D398" s="7" t="s">
         <v>511</v>
@@ -14161,7 +14161,7 @@
         <v>841</v>
       </c>
       <c r="C399" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D399" s="7" t="s">
         <v>418</v>
@@ -14184,7 +14184,7 @@
         <v>849</v>
       </c>
       <c r="C400" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D400" s="7" t="s">
         <v>418</v>
@@ -14207,7 +14207,7 @@
         <v>856</v>
       </c>
       <c r="C401" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D401" s="7" t="s">
         <v>418</v>
@@ -14230,7 +14230,7 @@
         <v>858</v>
       </c>
       <c r="C402" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D402" s="7" t="s">
         <v>418</v>
@@ -14250,10 +14250,10 @@
         <v>401</v>
       </c>
       <c r="B403" s="7" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="C403" s="7" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D403" s="7" t="s">
         <v>418</v>
@@ -14271,7 +14271,7 @@
         <v>2</v>
       </c>
       <c r="J403" s="7" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="404" spans="1:10" x14ac:dyDescent="0.25">
@@ -14282,7 +14282,7 @@
         <v>444</v>
       </c>
       <c r="C404" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D404" s="7" t="s">
         <v>418</v>
@@ -14311,7 +14311,7 @@
         <v>473</v>
       </c>
       <c r="C405" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D405" s="7" t="s">
         <v>418</v>
@@ -14343,7 +14343,7 @@
         <v>479</v>
       </c>
       <c r="C406" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D406" s="7" t="s">
         <v>418</v>
@@ -14375,7 +14375,7 @@
         <v>428</v>
       </c>
       <c r="C407" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D407" s="7" t="s">
         <v>418</v>
@@ -14407,7 +14407,7 @@
         <v>424</v>
       </c>
       <c r="C408" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D408" s="7" t="s">
         <v>418</v>
@@ -14439,7 +14439,7 @@
         <v>426</v>
       </c>
       <c r="C409" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D409" s="7" t="s">
         <v>418</v>
@@ -14471,7 +14471,7 @@
         <v>430</v>
       </c>
       <c r="C410" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D410" s="7" t="s">
         <v>418</v>
@@ -14503,7 +14503,7 @@
         <v>434</v>
       </c>
       <c r="C411" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D411" s="7" t="s">
         <v>418</v>
@@ -14532,7 +14532,7 @@
         <v>510</v>
       </c>
       <c r="C412" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D412" s="7" t="s">
         <v>511</v>
@@ -14561,7 +14561,7 @@
         <v>417</v>
       </c>
       <c r="C413" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D413" s="7" t="s">
         <v>418</v>
@@ -14593,7 +14593,7 @@
         <v>420</v>
       </c>
       <c r="C414" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D414" s="7" t="s">
         <v>418</v>
@@ -14622,7 +14622,7 @@
         <v>468</v>
       </c>
       <c r="C415" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D415" s="7" t="s">
         <v>418</v>
@@ -14651,7 +14651,7 @@
         <v>440</v>
       </c>
       <c r="C416" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D416" s="7" t="s">
         <v>418</v>
@@ -14680,7 +14680,7 @@
         <v>450</v>
       </c>
       <c r="C417" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D417" s="7" t="s">
         <v>418</v>
@@ -14709,7 +14709,7 @@
         <v>459</v>
       </c>
       <c r="C418" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D418" s="7" t="s">
         <v>418</v>
@@ -14738,7 +14738,7 @@
         <v>436</v>
       </c>
       <c r="C419" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D419" s="7" t="s">
         <v>418</v>
@@ -14767,7 +14767,7 @@
         <v>453</v>
       </c>
       <c r="C420" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D420" s="7" t="s">
         <v>418</v>
@@ -14796,7 +14796,7 @@
         <v>438</v>
       </c>
       <c r="C421" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D421" s="7" t="s">
         <v>418</v>
@@ -14825,7 +14825,7 @@
         <v>515</v>
       </c>
       <c r="C422" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D422" s="7" t="s">
         <v>511</v>
@@ -14854,7 +14854,7 @@
         <v>518</v>
       </c>
       <c r="C423" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D423" s="7" t="s">
         <v>511</v>
@@ -14883,7 +14883,7 @@
         <v>461</v>
       </c>
       <c r="C424" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D424" s="7" t="s">
         <v>418</v>
@@ -14915,7 +14915,7 @@
         <v>513</v>
       </c>
       <c r="C425" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D425" s="7" t="s">
         <v>511</v>
@@ -14944,7 +14944,7 @@
         <v>485</v>
       </c>
       <c r="C426" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D426" s="7" t="s">
         <v>418</v>
@@ -14973,7 +14973,7 @@
         <v>481</v>
       </c>
       <c r="C427" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D427" s="7" t="s">
         <v>418</v>
@@ -15005,7 +15005,7 @@
         <v>455</v>
       </c>
       <c r="C428" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D428" s="7" t="s">
         <v>418</v>
@@ -15037,7 +15037,7 @@
         <v>154</v>
       </c>
       <c r="C429" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D429" s="7" t="s">
         <v>418</v>
@@ -15069,7 +15069,7 @@
         <v>517</v>
       </c>
       <c r="C430" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D430" s="7" t="s">
         <v>511</v>
@@ -15098,7 +15098,7 @@
         <v>520</v>
       </c>
       <c r="C431" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D431" s="7" t="s">
         <v>511</v>
@@ -15127,7 +15127,7 @@
         <v>463</v>
       </c>
       <c r="C432" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D432" s="7" t="s">
         <v>418</v>
@@ -15156,7 +15156,7 @@
         <v>471</v>
       </c>
       <c r="C433" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D433" s="7" t="s">
         <v>418</v>
@@ -15188,7 +15188,7 @@
         <v>457</v>
       </c>
       <c r="C434" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D434" s="7" t="s">
         <v>418</v>
@@ -15220,7 +15220,7 @@
         <v>465</v>
       </c>
       <c r="C435" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D435" s="7" t="s">
         <v>418</v>
@@ -15252,7 +15252,7 @@
         <v>446</v>
       </c>
       <c r="C436" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D436" s="7" t="s">
         <v>418</v>
@@ -15281,7 +15281,7 @@
         <v>448</v>
       </c>
       <c r="C437" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D437" s="7" t="s">
         <v>418</v>
@@ -15310,7 +15310,7 @@
         <v>477</v>
       </c>
       <c r="C438" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D438" s="7" t="s">
         <v>418</v>
@@ -15342,7 +15342,7 @@
         <v>491</v>
       </c>
       <c r="C439" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D439" s="7" t="s">
         <v>418</v>
@@ -15371,7 +15371,7 @@
         <v>489</v>
       </c>
       <c r="C440" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D440" s="7" t="s">
         <v>418</v>
@@ -15403,7 +15403,7 @@
         <v>483</v>
       </c>
       <c r="C441" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D441" s="7" t="s">
         <v>418</v>
@@ -15432,7 +15432,7 @@
         <v>487</v>
       </c>
       <c r="C442" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D442" s="7" t="s">
         <v>418</v>
@@ -15464,7 +15464,7 @@
         <v>523</v>
       </c>
       <c r="C443" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D443" s="7" t="s">
         <v>511</v>
@@ -15493,7 +15493,7 @@
         <v>522</v>
       </c>
       <c r="C444" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D444" s="7" t="s">
         <v>511</v>
@@ -15522,7 +15522,7 @@
         <v>499</v>
       </c>
       <c r="C445" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D445" s="7" t="s">
         <v>418</v>
@@ -15551,7 +15551,7 @@
         <v>503</v>
       </c>
       <c r="C446" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D446" s="7" t="s">
         <v>418</v>
@@ -15583,7 +15583,7 @@
         <v>501</v>
       </c>
       <c r="C447" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D447" s="7" t="s">
         <v>418</v>
@@ -15612,7 +15612,7 @@
         <v>525</v>
       </c>
       <c r="C448" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D448" s="7" t="s">
         <v>511</v>
@@ -15641,7 +15641,7 @@
         <v>524</v>
       </c>
       <c r="C449" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D449" s="7" t="s">
         <v>511</v>
@@ -15670,7 +15670,7 @@
         <v>508</v>
       </c>
       <c r="C450" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D450" s="7" t="s">
         <v>418</v>
@@ -15702,7 +15702,7 @@
         <v>833</v>
       </c>
       <c r="C451" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D451" s="7" t="s">
         <v>418</v>
@@ -15725,7 +15725,7 @@
         <v>835</v>
       </c>
       <c r="C452" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D452" s="7" t="s">
         <v>418</v>
@@ -15748,7 +15748,7 @@
         <v>837</v>
       </c>
       <c r="C453" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D453" s="7" t="s">
         <v>418</v>
@@ -15771,7 +15771,7 @@
         <v>839</v>
       </c>
       <c r="C454" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D454" s="7" t="s">
         <v>418</v>
@@ -15794,7 +15794,7 @@
         <v>843</v>
       </c>
       <c r="C455" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D455" s="7" t="s">
         <v>418</v>
@@ -15817,7 +15817,7 @@
         <v>845</v>
       </c>
       <c r="C456" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D456" s="7" t="s">
         <v>418</v>
@@ -15840,7 +15840,7 @@
         <v>847</v>
       </c>
       <c r="C457" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D457" s="7" t="s">
         <v>418</v>
@@ -15863,7 +15863,7 @@
         <v>852</v>
       </c>
       <c r="C458" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D458" s="7" t="s">
         <v>418</v>
@@ -15886,7 +15886,7 @@
         <v>854</v>
       </c>
       <c r="C459" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D459" s="7" t="s">
         <v>418</v>
@@ -15909,7 +15909,7 @@
         <v>862</v>
       </c>
       <c r="C460" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D460" s="7" t="s">
         <v>418</v>
@@ -15932,7 +15932,7 @@
         <v>864</v>
       </c>
       <c r="C461" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D461" s="7" t="s">
         <v>418</v>
@@ -15955,7 +15955,7 @@
         <v>866</v>
       </c>
       <c r="C462" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D462" s="7" t="s">
         <v>418</v>
@@ -15978,7 +15978,7 @@
         <v>868</v>
       </c>
       <c r="C463" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D463" s="7" t="s">
         <v>418</v>
@@ -16001,7 +16001,7 @@
         <v>870</v>
       </c>
       <c r="C464" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D464" s="7" t="s">
         <v>418</v>
@@ -16024,7 +16024,7 @@
         <v>872</v>
       </c>
       <c r="C465" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D465" s="7" t="s">
         <v>418</v>
@@ -16047,7 +16047,7 @@
         <v>874</v>
       </c>
       <c r="C466" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D466" s="7" t="s">
         <v>511</v>
@@ -16070,7 +16070,7 @@
         <v>880</v>
       </c>
       <c r="C467" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D467" s="7" t="s">
         <v>511</v>
@@ -16093,7 +16093,7 @@
         <v>884</v>
       </c>
       <c r="C468" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D468" s="7" t="s">
         <v>511</v>
@@ -16113,10 +16113,10 @@
         <v>467</v>
       </c>
       <c r="B469" s="7" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C469" s="7" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D469" s="7" t="s">
         <v>418</v>
@@ -16134,7 +16134,7 @@
         <v>3</v>
       </c>
       <c r="J469" s="7" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="470" spans="1:10" x14ac:dyDescent="0.25">
@@ -16142,10 +16142,10 @@
         <v>468</v>
       </c>
       <c r="B470" s="7" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C470" s="7" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D470" s="7" t="s">
         <v>418</v>
@@ -16163,7 +16163,7 @@
         <v>2</v>
       </c>
       <c r="J470" s="7" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="471" spans="1:10" x14ac:dyDescent="0.25">
@@ -16171,10 +16171,10 @@
         <v>469</v>
       </c>
       <c r="B471" s="7" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C471" s="7" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D471" s="7" t="s">
         <v>418</v>
@@ -16192,7 +16192,7 @@
         <v>8</v>
       </c>
       <c r="J471" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="472" spans="1:10" x14ac:dyDescent="0.25">
@@ -16200,10 +16200,10 @@
         <v>470</v>
       </c>
       <c r="B472" s="7" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C472" s="7" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D472" s="7" t="s">
         <v>511</v>
@@ -16229,10 +16229,10 @@
         <v>471</v>
       </c>
       <c r="B473" s="7" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C473" s="7" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D473" s="7" t="s">
         <v>511</v>
@@ -16258,13 +16258,13 @@
         <v>472</v>
       </c>
       <c r="B474" s="7" t="s">
+        <v>925</v>
+      </c>
+      <c r="C474" s="7" t="s">
+        <v>921</v>
+      </c>
+      <c r="D474" s="7" t="s">
         <v>926</v>
-      </c>
-      <c r="C474" s="7" t="s">
-        <v>922</v>
-      </c>
-      <c r="D474" s="7" t="s">
-        <v>927</v>
       </c>
       <c r="F474" s="7" t="s">
         <v>5</v>
@@ -16287,7 +16287,7 @@
         <v>4</v>
       </c>
       <c r="C475" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D475" s="7" t="s">
         <v>418</v>
@@ -16316,7 +16316,7 @@
         <v>4</v>
       </c>
       <c r="C476" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D476" s="7" t="s">
         <v>418</v>
@@ -16345,7 +16345,7 @@
         <v>538</v>
       </c>
       <c r="C477" s="7" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D477" s="7" t="s">
         <v>418</v>
@@ -16368,7 +16368,7 @@
         <v>422</v>
       </c>
       <c r="C478" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D478" s="7" t="s">
         <v>418</v>
@@ -16397,7 +16397,7 @@
         <v>432</v>
       </c>
       <c r="C479" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D479" s="7" t="s">
         <v>418</v>
@@ -16426,7 +16426,7 @@
         <v>440</v>
       </c>
       <c r="C480" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D480" s="7" t="s">
         <v>418</v>
@@ -16455,7 +16455,7 @@
         <v>440</v>
       </c>
       <c r="C481" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D481" s="7" t="s">
         <v>418</v>
@@ -16484,7 +16484,7 @@
         <v>485</v>
       </c>
       <c r="C482" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D482" s="7" t="s">
         <v>511</v>

</xml_diff>

<commit_message>
Updated card info for Patch 1.2.0.6485
</commit_message>
<xml_diff>
--- a/card_info.xlsx
+++ b/card_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="28665" windowHeight="12750"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="19380" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="cards" sheetId="2" r:id="rId1"/>
@@ -3105,42 +3105,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF0FAF03"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF198EFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFAB48EE"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF07000"/>
-      </font>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF0FAF03"/>
@@ -3516,8 +3481,8 @@
   <dimension ref="A1:K566"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5611,13 +5576,13 @@
         <v>20</v>
       </c>
       <c r="H62" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I62" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J62" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K62" s="2" t="s">
         <v>25</v>
@@ -7782,7 +7747,7 @@
       </c>
       <c r="G127" s="2"/>
       <c r="H127" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I127" s="1">
         <v>6</v>
@@ -20409,16 +20374,16 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Legendary"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Epic"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Rare"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Common"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23264,16 +23229,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A565">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Legendary"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Epic"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Rare"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Common"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added new cards from The League of Explorers
</commit_message>
<xml_diff>
--- a/card_info.xlsx
+++ b/card_info.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5596" uniqueCount="1718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5947" uniqueCount="1827">
   <si>
     <t>Keeper of the Grove</t>
   </si>
@@ -5176,6 +5176,333 @@
   </si>
   <si>
     <t>Your Charge minions have +1 Attack.</t>
+  </si>
+  <si>
+    <t>Murloc Tinyfin</t>
+  </si>
+  <si>
+    <t>The League of Explorers</t>
+  </si>
+  <si>
+    <t>Huge Toad</t>
+  </si>
+  <si>
+    <t>Deathrattle: Deal 1 damage to a random enemy.</t>
+  </si>
+  <si>
+    <t>Jeweled Scarab</t>
+  </si>
+  <si>
+    <t>Battlecry: Discover a 3-Cost card.</t>
+  </si>
+  <si>
+    <t>Tomb Spider</t>
+  </si>
+  <si>
+    <t>Battlecry: Discover a Beast.</t>
+  </si>
+  <si>
+    <t>Gorillabot A-3</t>
+  </si>
+  <si>
+    <t>Battlecry: If you control another Mech. Discover a Mech.</t>
+  </si>
+  <si>
+    <t>Anubisath Sentinel</t>
+  </si>
+  <si>
+    <t>Deathrattle: Give a random friendly minion +3/+3.</t>
+  </si>
+  <si>
+    <t>Fossilized Devilsaur</t>
+  </si>
+  <si>
+    <t>Battlecry: If you control a Beast, gain Taunt.</t>
+  </si>
+  <si>
+    <t>Ancient Shade</t>
+  </si>
+  <si>
+    <t>Battlecry: Shuffle an 'Ancient Curse' into your deck that deals 7 damage to you when drawn.</t>
+  </si>
+  <si>
+    <t>Eerie Statue</t>
+  </si>
+  <si>
+    <t>Can't attack unless it's the only minion in the battlefield.</t>
+  </si>
+  <si>
+    <t>Summoning Stone</t>
+  </si>
+  <si>
+    <t>Whenever you cast a spell, summon a random minion of the same Cost.</t>
+  </si>
+  <si>
+    <t>Wobbling Runts</t>
+  </si>
+  <si>
+    <t>Deathrattle: Summon three 2/2 Runts.</t>
+  </si>
+  <si>
+    <t>Djinni of Zephyrs</t>
+  </si>
+  <si>
+    <t>After you cast a spell on another friendly minion, cast a copy of it on this one.</t>
+  </si>
+  <si>
+    <t>Naga Sea Witch</t>
+  </si>
+  <si>
+    <t>Your cards cost (5).</t>
+  </si>
+  <si>
+    <t>Sir Finley Mrrgglton</t>
+  </si>
+  <si>
+    <t>Battlecry: Discover a new basic Hero Power.</t>
+  </si>
+  <si>
+    <t>Brann Bronzebeard</t>
+  </si>
+  <si>
+    <t>Your Battlecries trigger twice.</t>
+  </si>
+  <si>
+    <t>Elise Starseeker</t>
+  </si>
+  <si>
+    <t>Battlecry: Shuffle the 'Map to the Golden Monkey' into your deck.</t>
+  </si>
+  <si>
+    <t>Reno Jackson</t>
+  </si>
+  <si>
+    <t>Battlecry: If your deck contains no more than 1 of any card, fully heal your hero.</t>
+  </si>
+  <si>
+    <t>Arch-Thief Rafaam</t>
+  </si>
+  <si>
+    <t>Battlecry: Discover a powerful Artifact.</t>
+  </si>
+  <si>
+    <t>Grumbly Runt</t>
+  </si>
+  <si>
+    <t>Rascally Runt</t>
+  </si>
+  <si>
+    <t>Wily Runt</t>
+  </si>
+  <si>
+    <t>Mummy Zombie</t>
+  </si>
+  <si>
+    <t>Golden Monkey</t>
+  </si>
+  <si>
+    <t>Taunt. Battlecry: Replace your hand and deck with Legendary minions.</t>
+  </si>
+  <si>
+    <t>Mounted Raptor</t>
+  </si>
+  <si>
+    <t>Deathrattle: Summon a random 1-Cost minion.</t>
+  </si>
+  <si>
+    <t>Jungle Moonkin</t>
+  </si>
+  <si>
+    <t>Desert Camel</t>
+  </si>
+  <si>
+    <t>Battlecry: Put a 1-Cost minion from each deck into the battlefield.</t>
+  </si>
+  <si>
+    <t>Ethereal Conjurer</t>
+  </si>
+  <si>
+    <t>Battlecry: Discover a spell.</t>
+  </si>
+  <si>
+    <t>Animated Armor</t>
+  </si>
+  <si>
+    <t>Your hero can only take 1 damage at a time.</t>
+  </si>
+  <si>
+    <t>Keeper of Uldaman</t>
+  </si>
+  <si>
+    <t>Battlecry: Set a minion's Attack and Health to 3.</t>
+  </si>
+  <si>
+    <t>Museum Curator</t>
+  </si>
+  <si>
+    <t>Battlecry: Discover a Deathrattle card.</t>
+  </si>
+  <si>
+    <t>Pit Snake</t>
+  </si>
+  <si>
+    <t>Tomb Pillager</t>
+  </si>
+  <si>
+    <t>Deathrattle: Add a Coin to your hand.</t>
+  </si>
+  <si>
+    <t>Unearthed Raptor</t>
+  </si>
+  <si>
+    <t>Battlecry: Choose a friendly minion. Gain a copy of its Deathrattle effect.</t>
+  </si>
+  <si>
+    <t>Tunnel Trogg</t>
+  </si>
+  <si>
+    <t>Whenever you Overload, gain +1 Attack per locked Mana Crystal.</t>
+  </si>
+  <si>
+    <t>Rumbling Elemental</t>
+  </si>
+  <si>
+    <t>After you play a Battlecry minion, deal 2 damage to a random enemy.</t>
+  </si>
+  <si>
+    <t>Dark Peddler</t>
+  </si>
+  <si>
+    <t>Battlecry: Discover a 1-Cost card.</t>
+  </si>
+  <si>
+    <t>Reliquary Seeker</t>
+  </si>
+  <si>
+    <t>Battlecry: If you have 6 other minions, gian +4/+4.</t>
+  </si>
+  <si>
+    <t>Fierce Monkey</t>
+  </si>
+  <si>
+    <t>Obsidian Destroyer</t>
+  </si>
+  <si>
+    <t>At the end of your turn, summon a 1/1 Scarab with Taunt.</t>
+  </si>
+  <si>
+    <t>Scarab</t>
+  </si>
+  <si>
+    <t>Ancient Curse</t>
+  </si>
+  <si>
+    <t>When you draw this, take 7 damage and draw a card.</t>
+  </si>
+  <si>
+    <t>Map to the Golden Monkey</t>
+  </si>
+  <si>
+    <t>Shuffle the Golden Monkey into your deck. Draw a card.</t>
+  </si>
+  <si>
+    <t>Mirror of Doom</t>
+  </si>
+  <si>
+    <t>Fill your board with 3/3 Mummy Zombies.</t>
+  </si>
+  <si>
+    <t>Timepiece of Horror</t>
+  </si>
+  <si>
+    <t>Deal 10 damage randomly split among all enemies.</t>
+  </si>
+  <si>
+    <t>Lantern of Power</t>
+  </si>
+  <si>
+    <t>Give a minion +10/+10.</t>
+  </si>
+  <si>
+    <t>Raven Idol</t>
+  </si>
+  <si>
+    <t>Choose One - Discover a minion; or Discover a spell.</t>
+  </si>
+  <si>
+    <t>Dart Trap</t>
+  </si>
+  <si>
+    <t>Secret: When an opposing Hero Power is used, deal 5 damage to a random enemy.</t>
+  </si>
+  <si>
+    <t>Explorer's Hat</t>
+  </si>
+  <si>
+    <t>Give a minion +1/+1 and "Deathrattle: Add an Explorer's Hat to your hand."</t>
+  </si>
+  <si>
+    <t>Forgotten Torch</t>
+  </si>
+  <si>
+    <t>Deal 3 damage. Shuffle a 'Roaring Torch' into your deck that deals 6 damage.</t>
+  </si>
+  <si>
+    <t>Sacred Trial</t>
+  </si>
+  <si>
+    <t>Secret: When your opponent has at least 3 minions and plays another, destroy it.</t>
+  </si>
+  <si>
+    <t>Anyfin Can Happen</t>
+  </si>
+  <si>
+    <t>Summon 7 Murlocs that died this game.</t>
+  </si>
+  <si>
+    <t>Entomb</t>
+  </si>
+  <si>
+    <t>Choose an enemy minion. Shuffle it into your deck.</t>
+  </si>
+  <si>
+    <t>Excavated Evil</t>
+  </si>
+  <si>
+    <t>Deal 3 damage to all minions. Shuffle this card into your opponent's deck.</t>
+  </si>
+  <si>
+    <t>Everyfin is Awesome</t>
+  </si>
+  <si>
+    <t>Give your minions +2/+2. Costs (1) less for each Murloc you control.</t>
+  </si>
+  <si>
+    <t>Curse of Rafaam</t>
+  </si>
+  <si>
+    <t>Give your opponent a 'Cursed!' card. While they hold it, they take 2 damage on their turn.</t>
+  </si>
+  <si>
+    <t>Cursed!</t>
+  </si>
+  <si>
+    <t>While this is in your hand, take 2 damage at the start of your turn.</t>
+  </si>
+  <si>
+    <t>Roaring Torch</t>
+  </si>
+  <si>
+    <t>Discover a minion.</t>
+  </si>
+  <si>
+    <t>Discover a spell.</t>
+  </si>
+  <si>
+    <t>Cursed Blade</t>
+  </si>
+  <si>
+    <t>Double all damage dealt to your hero.</t>
   </si>
 </sst>
 </file>
@@ -5236,7 +5563,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FFF07000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFAB48EE"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF198EFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0FAF03"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFF07000"/>
@@ -5582,11 +5949,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K955"/>
+  <dimension ref="A1:K1015"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K100" sqref="K100"/>
+      <pane ySplit="1" topLeftCell="A963" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1015" sqref="B1015"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34696,12 +35063,1791 @@
         <v>2</v>
       </c>
     </row>
+    <row r="956" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A956" s="1">
+        <v>954</v>
+      </c>
+      <c r="B956" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C956" t="s">
+        <v>831</v>
+      </c>
+      <c r="D956" t="s">
+        <v>139</v>
+      </c>
+      <c r="E956" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F956" t="s">
+        <v>5</v>
+      </c>
+      <c r="G956" t="s">
+        <v>153</v>
+      </c>
+      <c r="H956">
+        <v>0</v>
+      </c>
+      <c r="I956">
+        <v>1</v>
+      </c>
+      <c r="J956">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="957" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A957" s="1">
+        <v>955</v>
+      </c>
+      <c r="B957" t="s">
+        <v>1720</v>
+      </c>
+      <c r="C957" t="s">
+        <v>831</v>
+      </c>
+      <c r="D957" t="s">
+        <v>139</v>
+      </c>
+      <c r="E957" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F957" t="s">
+        <v>5</v>
+      </c>
+      <c r="G957" t="s">
+        <v>20</v>
+      </c>
+      <c r="H957">
+        <v>2</v>
+      </c>
+      <c r="I957">
+        <v>3</v>
+      </c>
+      <c r="J957">
+        <v>2</v>
+      </c>
+      <c r="K957" t="s">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="958" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A958" s="1">
+        <v>956</v>
+      </c>
+      <c r="B958" t="s">
+        <v>1722</v>
+      </c>
+      <c r="C958" t="s">
+        <v>831</v>
+      </c>
+      <c r="D958" t="s">
+        <v>139</v>
+      </c>
+      <c r="E958" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F958" t="s">
+        <v>5</v>
+      </c>
+      <c r="G958" t="s">
+        <v>20</v>
+      </c>
+      <c r="H958">
+        <v>2</v>
+      </c>
+      <c r="I958">
+        <v>1</v>
+      </c>
+      <c r="J958">
+        <v>1</v>
+      </c>
+      <c r="K958" t="s">
+        <v>1723</v>
+      </c>
+    </row>
+    <row r="959" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A959" s="1">
+        <v>957</v>
+      </c>
+      <c r="B959" t="s">
+        <v>1724</v>
+      </c>
+      <c r="C959" t="s">
+        <v>831</v>
+      </c>
+      <c r="D959" t="s">
+        <v>139</v>
+      </c>
+      <c r="E959" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F959" t="s">
+        <v>5</v>
+      </c>
+      <c r="G959" t="s">
+        <v>20</v>
+      </c>
+      <c r="H959">
+        <v>4</v>
+      </c>
+      <c r="I959">
+        <v>3</v>
+      </c>
+      <c r="J959">
+        <v>3</v>
+      </c>
+      <c r="K959" t="s">
+        <v>1725</v>
+      </c>
+    </row>
+    <row r="960" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A960" s="1">
+        <v>958</v>
+      </c>
+      <c r="B960" t="s">
+        <v>1726</v>
+      </c>
+      <c r="C960" t="s">
+        <v>831</v>
+      </c>
+      <c r="D960" t="s">
+        <v>139</v>
+      </c>
+      <c r="E960" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F960" t="s">
+        <v>5</v>
+      </c>
+      <c r="G960" t="s">
+        <v>1004</v>
+      </c>
+      <c r="H960">
+        <v>4</v>
+      </c>
+      <c r="I960">
+        <v>3</v>
+      </c>
+      <c r="J960">
+        <v>4</v>
+      </c>
+      <c r="K960" t="s">
+        <v>1727</v>
+      </c>
+    </row>
+    <row r="961" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A961" s="1">
+        <v>959</v>
+      </c>
+      <c r="B961" t="s">
+        <v>1728</v>
+      </c>
+      <c r="C961" t="s">
+        <v>831</v>
+      </c>
+      <c r="D961" t="s">
+        <v>139</v>
+      </c>
+      <c r="E961" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F961" t="s">
+        <v>5</v>
+      </c>
+      <c r="H961">
+        <v>5</v>
+      </c>
+      <c r="I961">
+        <v>4</v>
+      </c>
+      <c r="J961">
+        <v>4</v>
+      </c>
+      <c r="K961" t="s">
+        <v>1729</v>
+      </c>
+    </row>
+    <row r="962" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A962" s="1">
+        <v>960</v>
+      </c>
+      <c r="B962" t="s">
+        <v>1730</v>
+      </c>
+      <c r="C962" t="s">
+        <v>831</v>
+      </c>
+      <c r="D962" t="s">
+        <v>139</v>
+      </c>
+      <c r="E962" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F962" t="s">
+        <v>5</v>
+      </c>
+      <c r="H962">
+        <v>8</v>
+      </c>
+      <c r="I962">
+        <v>8</v>
+      </c>
+      <c r="J962">
+        <v>8</v>
+      </c>
+      <c r="K962" t="s">
+        <v>1731</v>
+      </c>
+    </row>
+    <row r="963" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A963" s="1">
+        <v>961</v>
+      </c>
+      <c r="B963" t="s">
+        <v>1732</v>
+      </c>
+      <c r="C963" t="s">
+        <v>831</v>
+      </c>
+      <c r="D963" t="s">
+        <v>139</v>
+      </c>
+      <c r="E963" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F963" t="s">
+        <v>2</v>
+      </c>
+      <c r="H963">
+        <v>4</v>
+      </c>
+      <c r="I963">
+        <v>7</v>
+      </c>
+      <c r="J963">
+        <v>4</v>
+      </c>
+      <c r="K963" t="s">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="964" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A964" s="1">
+        <v>962</v>
+      </c>
+      <c r="B964" t="s">
+        <v>1734</v>
+      </c>
+      <c r="C964" t="s">
+        <v>831</v>
+      </c>
+      <c r="D964" t="s">
+        <v>139</v>
+      </c>
+      <c r="E964" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F964" t="s">
+        <v>2</v>
+      </c>
+      <c r="H964">
+        <v>4</v>
+      </c>
+      <c r="I964">
+        <v>7</v>
+      </c>
+      <c r="J964">
+        <v>7</v>
+      </c>
+      <c r="K964" t="s">
+        <v>1735</v>
+      </c>
+    </row>
+    <row r="965" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A965" s="1">
+        <v>963</v>
+      </c>
+      <c r="B965" t="s">
+        <v>1736</v>
+      </c>
+      <c r="C965" t="s">
+        <v>831</v>
+      </c>
+      <c r="D965" t="s">
+        <v>139</v>
+      </c>
+      <c r="E965" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F965" t="s">
+        <v>2</v>
+      </c>
+      <c r="H965">
+        <v>5</v>
+      </c>
+      <c r="I965">
+        <v>0</v>
+      </c>
+      <c r="J965">
+        <v>6</v>
+      </c>
+      <c r="K965" t="s">
+        <v>1737</v>
+      </c>
+    </row>
+    <row r="966" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A966" s="1">
+        <v>964</v>
+      </c>
+      <c r="B966" t="s">
+        <v>1738</v>
+      </c>
+      <c r="C966" t="s">
+        <v>831</v>
+      </c>
+      <c r="D966" t="s">
+        <v>139</v>
+      </c>
+      <c r="E966" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F966" t="s">
+        <v>2</v>
+      </c>
+      <c r="H966">
+        <v>6</v>
+      </c>
+      <c r="I966">
+        <v>2</v>
+      </c>
+      <c r="J966">
+        <v>6</v>
+      </c>
+      <c r="K966" t="s">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="967" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A967" s="1">
+        <v>965</v>
+      </c>
+      <c r="B967" t="s">
+        <v>1740</v>
+      </c>
+      <c r="C967" t="s">
+        <v>831</v>
+      </c>
+      <c r="D967" t="s">
+        <v>139</v>
+      </c>
+      <c r="E967" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F967" t="s">
+        <v>8</v>
+      </c>
+      <c r="H967">
+        <v>5</v>
+      </c>
+      <c r="I967">
+        <v>4</v>
+      </c>
+      <c r="J967">
+        <v>6</v>
+      </c>
+      <c r="K967" t="s">
+        <v>1741</v>
+      </c>
+    </row>
+    <row r="968" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A968" s="1">
+        <v>966</v>
+      </c>
+      <c r="B968" t="s">
+        <v>1742</v>
+      </c>
+      <c r="C968" t="s">
+        <v>831</v>
+      </c>
+      <c r="D968" t="s">
+        <v>139</v>
+      </c>
+      <c r="E968" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F968" t="s">
+        <v>8</v>
+      </c>
+      <c r="H968">
+        <v>5</v>
+      </c>
+      <c r="I968">
+        <v>5</v>
+      </c>
+      <c r="J968">
+        <v>5</v>
+      </c>
+      <c r="K968" t="s">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="969" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A969" s="1">
+        <v>967</v>
+      </c>
+      <c r="B969" t="s">
+        <v>1744</v>
+      </c>
+      <c r="C969" t="s">
+        <v>831</v>
+      </c>
+      <c r="D969" t="s">
+        <v>139</v>
+      </c>
+      <c r="E969" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F969" t="s">
+        <v>16</v>
+      </c>
+      <c r="G969" t="s">
+        <v>153</v>
+      </c>
+      <c r="H969">
+        <v>1</v>
+      </c>
+      <c r="I969">
+        <v>1</v>
+      </c>
+      <c r="J969">
+        <v>3</v>
+      </c>
+      <c r="K969" t="s">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="970" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A970" s="1">
+        <v>968</v>
+      </c>
+      <c r="B970" t="s">
+        <v>1746</v>
+      </c>
+      <c r="C970" t="s">
+        <v>831</v>
+      </c>
+      <c r="D970" t="s">
+        <v>139</v>
+      </c>
+      <c r="E970" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F970" t="s">
+        <v>16</v>
+      </c>
+      <c r="H970">
+        <v>3</v>
+      </c>
+      <c r="I970">
+        <v>2</v>
+      </c>
+      <c r="J970">
+        <v>4</v>
+      </c>
+      <c r="K970" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="971" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A971" s="1">
+        <v>969</v>
+      </c>
+      <c r="B971" t="s">
+        <v>1748</v>
+      </c>
+      <c r="C971" t="s">
+        <v>831</v>
+      </c>
+      <c r="D971" t="s">
+        <v>139</v>
+      </c>
+      <c r="E971" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F971" t="s">
+        <v>16</v>
+      </c>
+      <c r="H971">
+        <v>4</v>
+      </c>
+      <c r="I971">
+        <v>3</v>
+      </c>
+      <c r="J971">
+        <v>5</v>
+      </c>
+      <c r="K971" t="s">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="972" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A972" s="1">
+        <v>970</v>
+      </c>
+      <c r="B972" t="s">
+        <v>1750</v>
+      </c>
+      <c r="C972" t="s">
+        <v>831</v>
+      </c>
+      <c r="D972" t="s">
+        <v>139</v>
+      </c>
+      <c r="E972" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F972" t="s">
+        <v>16</v>
+      </c>
+      <c r="H972">
+        <v>6</v>
+      </c>
+      <c r="I972">
+        <v>4</v>
+      </c>
+      <c r="J972">
+        <v>6</v>
+      </c>
+      <c r="K972" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="973" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A973" s="1">
+        <v>971</v>
+      </c>
+      <c r="B973" t="s">
+        <v>1752</v>
+      </c>
+      <c r="C973" t="s">
+        <v>831</v>
+      </c>
+      <c r="D973" t="s">
+        <v>139</v>
+      </c>
+      <c r="E973" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F973" t="s">
+        <v>16</v>
+      </c>
+      <c r="H973">
+        <v>9</v>
+      </c>
+      <c r="I973">
+        <v>7</v>
+      </c>
+      <c r="J973">
+        <v>8</v>
+      </c>
+      <c r="K973" t="s">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="974" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A974" s="1">
+        <v>972</v>
+      </c>
+      <c r="B974" t="s">
+        <v>1754</v>
+      </c>
+      <c r="C974" t="s">
+        <v>831</v>
+      </c>
+      <c r="E974" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F974" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H974">
+        <v>2</v>
+      </c>
+      <c r="I974">
+        <v>2</v>
+      </c>
+      <c r="J974">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="975" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A975" s="1">
+        <v>973</v>
+      </c>
+      <c r="B975" t="s">
+        <v>1755</v>
+      </c>
+      <c r="C975" t="s">
+        <v>831</v>
+      </c>
+      <c r="E975" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F975" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H975">
+        <v>2</v>
+      </c>
+      <c r="I975">
+        <v>2</v>
+      </c>
+      <c r="J975">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="976" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A976" s="1">
+        <v>974</v>
+      </c>
+      <c r="B976" t="s">
+        <v>1756</v>
+      </c>
+      <c r="C976" t="s">
+        <v>831</v>
+      </c>
+      <c r="E976" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F976" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H976">
+        <v>2</v>
+      </c>
+      <c r="I976">
+        <v>2</v>
+      </c>
+      <c r="J976">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="977" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A977" s="1">
+        <v>975</v>
+      </c>
+      <c r="B977" t="s">
+        <v>1757</v>
+      </c>
+      <c r="C977" t="s">
+        <v>831</v>
+      </c>
+      <c r="E977" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F977" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H977">
+        <v>3</v>
+      </c>
+      <c r="I977">
+        <v>3</v>
+      </c>
+      <c r="J977">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="978" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A978" s="1">
+        <v>976</v>
+      </c>
+      <c r="B978" t="s">
+        <v>1758</v>
+      </c>
+      <c r="C978" t="s">
+        <v>831</v>
+      </c>
+      <c r="E978" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F978" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H978">
+        <v>4</v>
+      </c>
+      <c r="I978">
+        <v>6</v>
+      </c>
+      <c r="J978">
+        <v>6</v>
+      </c>
+      <c r="K978" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="979" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A979" s="1">
+        <v>977</v>
+      </c>
+      <c r="B979" t="s">
+        <v>1760</v>
+      </c>
+      <c r="C979" t="s">
+        <v>831</v>
+      </c>
+      <c r="D979" t="s">
+        <v>1</v>
+      </c>
+      <c r="E979" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F979" t="s">
+        <v>5</v>
+      </c>
+      <c r="G979" t="s">
+        <v>20</v>
+      </c>
+      <c r="H979">
+        <v>3</v>
+      </c>
+      <c r="I979">
+        <v>3</v>
+      </c>
+      <c r="J979">
+        <v>2</v>
+      </c>
+      <c r="K979" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="980" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A980" s="1">
+        <v>978</v>
+      </c>
+      <c r="B980" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C980" t="s">
+        <v>831</v>
+      </c>
+      <c r="D980" t="s">
+        <v>1</v>
+      </c>
+      <c r="E980" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F980" t="s">
+        <v>2</v>
+      </c>
+      <c r="G980" t="s">
+        <v>20</v>
+      </c>
+      <c r="H980">
+        <v>4</v>
+      </c>
+      <c r="I980">
+        <v>4</v>
+      </c>
+      <c r="J980">
+        <v>4</v>
+      </c>
+      <c r="K980" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="981" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A981" s="1">
+        <v>979</v>
+      </c>
+      <c r="B981" t="s">
+        <v>1763</v>
+      </c>
+      <c r="C981" t="s">
+        <v>831</v>
+      </c>
+      <c r="D981" t="s">
+        <v>19</v>
+      </c>
+      <c r="E981" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F981" t="s">
+        <v>5</v>
+      </c>
+      <c r="G981" t="s">
+        <v>20</v>
+      </c>
+      <c r="H981">
+        <v>3</v>
+      </c>
+      <c r="I981">
+        <v>2</v>
+      </c>
+      <c r="J981">
+        <v>4</v>
+      </c>
+      <c r="K981" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="982" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A982" s="1">
+        <v>980</v>
+      </c>
+      <c r="B982" t="s">
+        <v>1765</v>
+      </c>
+      <c r="C982" t="s">
+        <v>831</v>
+      </c>
+      <c r="D982" t="s">
+        <v>35</v>
+      </c>
+      <c r="E982" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F982" t="s">
+        <v>5</v>
+      </c>
+      <c r="H982">
+        <v>5</v>
+      </c>
+      <c r="I982">
+        <v>6</v>
+      </c>
+      <c r="J982">
+        <v>3</v>
+      </c>
+      <c r="K982" t="s">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="983" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A983" s="1">
+        <v>981</v>
+      </c>
+      <c r="B983" t="s">
+        <v>1767</v>
+      </c>
+      <c r="C983" t="s">
+        <v>831</v>
+      </c>
+      <c r="D983" t="s">
+        <v>35</v>
+      </c>
+      <c r="E983" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F983" t="s">
+        <v>2</v>
+      </c>
+      <c r="H983">
+        <v>4</v>
+      </c>
+      <c r="I983">
+        <v>4</v>
+      </c>
+      <c r="J983">
+        <v>4</v>
+      </c>
+      <c r="K983" t="s">
+        <v>1768</v>
+      </c>
+    </row>
+    <row r="984" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A984" s="1">
+        <v>982</v>
+      </c>
+      <c r="B984" t="s">
+        <v>1769</v>
+      </c>
+      <c r="C984" t="s">
+        <v>831</v>
+      </c>
+      <c r="D984" t="s">
+        <v>48</v>
+      </c>
+      <c r="E984" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F984" t="s">
+        <v>5</v>
+      </c>
+      <c r="H984">
+        <v>4</v>
+      </c>
+      <c r="I984">
+        <v>3</v>
+      </c>
+      <c r="J984">
+        <v>4</v>
+      </c>
+      <c r="K984" t="s">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="985" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A985" s="1">
+        <v>983</v>
+      </c>
+      <c r="B985" t="s">
+        <v>1771</v>
+      </c>
+      <c r="C985" t="s">
+        <v>831</v>
+      </c>
+      <c r="D985" t="s">
+        <v>57</v>
+      </c>
+      <c r="E985" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F985" t="s">
+        <v>5</v>
+      </c>
+      <c r="H985">
+        <v>2</v>
+      </c>
+      <c r="I985">
+        <v>1</v>
+      </c>
+      <c r="J985">
+        <v>2</v>
+      </c>
+      <c r="K985" t="s">
+        <v>1772</v>
+      </c>
+    </row>
+    <row r="986" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A986" s="1">
+        <v>984</v>
+      </c>
+      <c r="B986" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C986" t="s">
+        <v>831</v>
+      </c>
+      <c r="D986" t="s">
+        <v>72</v>
+      </c>
+      <c r="E986" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F986" t="s">
+        <v>5</v>
+      </c>
+      <c r="G986" t="s">
+        <v>20</v>
+      </c>
+      <c r="H986">
+        <v>1</v>
+      </c>
+      <c r="I986">
+        <v>2</v>
+      </c>
+      <c r="J986">
+        <v>1</v>
+      </c>
+      <c r="K986" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="987" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A987" s="1">
+        <v>985</v>
+      </c>
+      <c r="B987" t="s">
+        <v>1774</v>
+      </c>
+      <c r="C987" t="s">
+        <v>831</v>
+      </c>
+      <c r="D987" t="s">
+        <v>72</v>
+      </c>
+      <c r="E987" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F987" t="s">
+        <v>5</v>
+      </c>
+      <c r="H987">
+        <v>4</v>
+      </c>
+      <c r="I987">
+        <v>5</v>
+      </c>
+      <c r="J987">
+        <v>4</v>
+      </c>
+      <c r="K987" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="988" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A988" s="1">
+        <v>986</v>
+      </c>
+      <c r="B988" t="s">
+        <v>1776</v>
+      </c>
+      <c r="C988" t="s">
+        <v>831</v>
+      </c>
+      <c r="D988" t="s">
+        <v>72</v>
+      </c>
+      <c r="E988" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F988" t="s">
+        <v>2</v>
+      </c>
+      <c r="H988">
+        <v>3</v>
+      </c>
+      <c r="I988">
+        <v>3</v>
+      </c>
+      <c r="J988">
+        <v>4</v>
+      </c>
+      <c r="K988" t="s">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="989" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A989" s="1">
+        <v>987</v>
+      </c>
+      <c r="B989" t="s">
+        <v>1778</v>
+      </c>
+      <c r="C989" t="s">
+        <v>831</v>
+      </c>
+      <c r="D989" t="s">
+        <v>85</v>
+      </c>
+      <c r="E989" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F989" t="s">
+        <v>5</v>
+      </c>
+      <c r="H989">
+        <v>1</v>
+      </c>
+      <c r="I989">
+        <v>1</v>
+      </c>
+      <c r="J989">
+        <v>3</v>
+      </c>
+      <c r="K989" t="s">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="990" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A990" s="1">
+        <v>988</v>
+      </c>
+      <c r="B990" t="s">
+        <v>1780</v>
+      </c>
+      <c r="C990" t="s">
+        <v>831</v>
+      </c>
+      <c r="D990" t="s">
+        <v>85</v>
+      </c>
+      <c r="E990" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F990" t="s">
+        <v>5</v>
+      </c>
+      <c r="H990">
+        <v>4</v>
+      </c>
+      <c r="I990">
+        <v>2</v>
+      </c>
+      <c r="J990">
+        <v>6</v>
+      </c>
+      <c r="K990" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="991" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A991" s="1">
+        <v>989</v>
+      </c>
+      <c r="B991" t="s">
+        <v>1782</v>
+      </c>
+      <c r="C991" t="s">
+        <v>831</v>
+      </c>
+      <c r="D991" t="s">
+        <v>103</v>
+      </c>
+      <c r="E991" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F991" t="s">
+        <v>5</v>
+      </c>
+      <c r="H991">
+        <v>2</v>
+      </c>
+      <c r="I991">
+        <v>2</v>
+      </c>
+      <c r="J991">
+        <v>2</v>
+      </c>
+      <c r="K991" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="992" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A992" s="1">
+        <v>990</v>
+      </c>
+      <c r="B992" t="s">
+        <v>1784</v>
+      </c>
+      <c r="C992" t="s">
+        <v>831</v>
+      </c>
+      <c r="D992" t="s">
+        <v>103</v>
+      </c>
+      <c r="E992" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F992" t="s">
+        <v>2</v>
+      </c>
+      <c r="H992">
+        <v>1</v>
+      </c>
+      <c r="I992">
+        <v>1</v>
+      </c>
+      <c r="J992">
+        <v>1</v>
+      </c>
+      <c r="K992" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="993" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A993" s="1">
+        <v>991</v>
+      </c>
+      <c r="B993" t="s">
+        <v>1786</v>
+      </c>
+      <c r="C993" t="s">
+        <v>831</v>
+      </c>
+      <c r="D993" t="s">
+        <v>126</v>
+      </c>
+      <c r="E993" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F993" t="s">
+        <v>5</v>
+      </c>
+      <c r="G993" t="s">
+        <v>20</v>
+      </c>
+      <c r="H993">
+        <v>3</v>
+      </c>
+      <c r="I993">
+        <v>3</v>
+      </c>
+      <c r="J993">
+        <v>4</v>
+      </c>
+      <c r="K993" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="994" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A994" s="1">
+        <v>992</v>
+      </c>
+      <c r="B994" t="s">
+        <v>1787</v>
+      </c>
+      <c r="C994" t="s">
+        <v>831</v>
+      </c>
+      <c r="D994" t="s">
+        <v>126</v>
+      </c>
+      <c r="E994" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F994" t="s">
+        <v>5</v>
+      </c>
+      <c r="H994">
+        <v>7</v>
+      </c>
+      <c r="I994">
+        <v>7</v>
+      </c>
+      <c r="J994">
+        <v>7</v>
+      </c>
+      <c r="K994" t="s">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="995" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A995" s="1">
+        <v>993</v>
+      </c>
+      <c r="B995" t="s">
+        <v>1789</v>
+      </c>
+      <c r="C995" t="s">
+        <v>831</v>
+      </c>
+      <c r="E995" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F995" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H995">
+        <v>1</v>
+      </c>
+      <c r="I995">
+        <v>1</v>
+      </c>
+      <c r="J995">
+        <v>1</v>
+      </c>
+      <c r="K995" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="996" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A996" s="1">
+        <v>994</v>
+      </c>
+      <c r="B996" t="s">
+        <v>1790</v>
+      </c>
+      <c r="C996" t="s">
+        <v>989</v>
+      </c>
+      <c r="E996" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F996" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H996">
+        <v>0</v>
+      </c>
+      <c r="K996" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="997" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A997" s="1">
+        <v>995</v>
+      </c>
+      <c r="B997" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C997" t="s">
+        <v>989</v>
+      </c>
+      <c r="E997" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F997" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H997">
+        <v>2</v>
+      </c>
+      <c r="K997" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="998" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A998" s="1">
+        <v>996</v>
+      </c>
+      <c r="B998" t="s">
+        <v>1794</v>
+      </c>
+      <c r="C998" t="s">
+        <v>989</v>
+      </c>
+      <c r="E998" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F998" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H998">
+        <v>10</v>
+      </c>
+      <c r="K998" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="999" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A999" s="1">
+        <v>997</v>
+      </c>
+      <c r="B999" t="s">
+        <v>1796</v>
+      </c>
+      <c r="C999" t="s">
+        <v>989</v>
+      </c>
+      <c r="E999" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F999" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H999">
+        <v>10</v>
+      </c>
+      <c r="K999" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1000" s="1">
+        <v>998</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>1798</v>
+      </c>
+      <c r="C1000" t="s">
+        <v>989</v>
+      </c>
+      <c r="E1000" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1000" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H1000">
+        <v>10</v>
+      </c>
+      <c r="K1000" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1001" s="1">
+        <v>999</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C1001" t="s">
+        <v>989</v>
+      </c>
+      <c r="D1001" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1001" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1001" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1001">
+        <v>1</v>
+      </c>
+      <c r="K1001" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1002" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>989</v>
+      </c>
+      <c r="D1002" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1002" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1002" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1002">
+        <v>2</v>
+      </c>
+      <c r="K1002" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1003" s="1">
+        <v>1001</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>989</v>
+      </c>
+      <c r="D1003" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1003" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1003" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1003">
+        <v>2</v>
+      </c>
+      <c r="K1003" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1004" s="1">
+        <v>1002</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>1806</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>989</v>
+      </c>
+      <c r="D1004" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1004" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1004" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1004">
+        <v>3</v>
+      </c>
+      <c r="K1004" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1005" s="1">
+        <v>1003</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>1808</v>
+      </c>
+      <c r="C1005" t="s">
+        <v>989</v>
+      </c>
+      <c r="D1005" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1005" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1005" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1005">
+        <v>1</v>
+      </c>
+      <c r="K1005" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1006" s="1">
+        <v>1004</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>1810</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>989</v>
+      </c>
+      <c r="D1006" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1006" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1006" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1006">
+        <v>10</v>
+      </c>
+      <c r="K1006" t="s">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1007" s="1">
+        <v>1005</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>1812</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>989</v>
+      </c>
+      <c r="D1007" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1007" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1007" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1007">
+        <v>6</v>
+      </c>
+      <c r="K1007" t="s">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1008" s="1">
+        <v>1006</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>1814</v>
+      </c>
+      <c r="C1008" t="s">
+        <v>989</v>
+      </c>
+      <c r="D1008" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1008" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1008" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1008">
+        <v>5</v>
+      </c>
+      <c r="K1008" t="s">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1009" s="1">
+        <v>1007</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>1816</v>
+      </c>
+      <c r="C1009" t="s">
+        <v>989</v>
+      </c>
+      <c r="D1009" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1009" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1009" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1009">
+        <v>7</v>
+      </c>
+      <c r="K1009" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1010" s="1">
+        <v>1008</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>989</v>
+      </c>
+      <c r="D1010" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1010" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1010" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1010">
+        <v>2</v>
+      </c>
+      <c r="K1010" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1011" s="1">
+        <v>1009</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C1011" t="s">
+        <v>989</v>
+      </c>
+      <c r="E1011" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1011" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H1011">
+        <v>2</v>
+      </c>
+      <c r="K1011" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1012" s="1">
+        <v>1010</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>1822</v>
+      </c>
+      <c r="C1012" t="s">
+        <v>989</v>
+      </c>
+      <c r="E1012" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1012" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H1012">
+        <v>3</v>
+      </c>
+      <c r="K1012" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1013" s="1">
+        <v>1011</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C1013" t="s">
+        <v>989</v>
+      </c>
+      <c r="E1013" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1013" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H1013">
+        <v>0</v>
+      </c>
+      <c r="K1013" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1014" s="1">
+        <v>1012</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C1014" t="s">
+        <v>989</v>
+      </c>
+      <c r="E1014" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1014" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H1014">
+        <v>0</v>
+      </c>
+      <c r="K1014" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1015" s="1">
+        <v>1013</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>1825</v>
+      </c>
+      <c r="C1015" t="s">
+        <v>832</v>
+      </c>
+      <c r="D1015" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1015" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F1015" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1015">
+        <v>1</v>
+      </c>
+      <c r="I1015">
+        <v>2</v>
+      </c>
+      <c r="J1015">
+        <v>3</v>
+      </c>
+      <c r="K1015" t="s">
+        <v>1826</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K955"/>
   <sortState ref="A2:K709">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="F1:F1048576 G905:G944 G950:G955">
+  <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="cellIs" dxfId="3" priority="18" operator="equal">
       <formula>"Common"</formula>
     </cfRule>

</xml_diff>